<commit_message>
Changed Month to "November"
</commit_message>
<xml_diff>
--- a/Dokumentation/Aquila_Zeitaufzeichnung.xlsx
+++ b/Dokumentation/Aquila_Zeitaufzeichnung.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="85">
   <si>
     <t>Arbeitspaket</t>
   </si>
@@ -838,12 +838,12 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:shape val="box"/>
-        <c:axId val="85827584"/>
-        <c:axId val="85829120"/>
+        <c:axId val="93102080"/>
+        <c:axId val="93103616"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="85827584"/>
+        <c:axId val="93102080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -852,7 +852,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85829120"/>
+        <c:crossAx val="93103616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -860,7 +860,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="85829120"/>
+        <c:axId val="93103616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -876,7 +876,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="85827584"/>
+        <c:crossAx val="93102080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -995,13 +995,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>12.5</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9</c:v>
+                  <c:v>11.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1017,12 +1017,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="40634240"/>
-        <c:axId val="40635776"/>
+        <c:axId val="93456256"/>
+        <c:axId val="93457792"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="40634240"/>
+        <c:axId val="93456256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1031,7 +1031,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40635776"/>
+        <c:crossAx val="93457792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1039,7 +1039,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40635776"/>
+        <c:axId val="93457792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1050,7 +1050,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40634240"/>
+        <c:crossAx val="93456256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1813,7 +1813,7 @@
       <c r="C35" s="54"/>
       <c r="D35" s="12">
         <f>SUM(Projektmanagement!I13,Software!I12,Website!I12,Schnittstellen!J11,'Testing &amp; Abschluss'!I13)</f>
-        <v>12.5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
@@ -1833,7 +1833,7 @@
       <c r="C37" s="50"/>
       <c r="D37" s="40">
         <f>SUM(Projektmanagement!I15,Software!I14,Website!I14,Schnittstellen!J13,'Testing &amp; Abschluss'!I15)</f>
-        <v>9</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2489,7 +2489,7 @@
   <dimension ref="A1:J68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2643,7 +2643,21 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D6" s="1"/>
+      <c r="A6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" s="1">
+        <v>41248</v>
+      </c>
+      <c r="E6" s="3">
+        <v>2.5</v>
+      </c>
       <c r="H6" s="63" t="s">
         <v>16</v>
       </c>
@@ -2654,7 +2668,21 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D7" s="8"/>
+      <c r="A7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="1">
+        <v>41248</v>
+      </c>
+      <c r="E7" s="3">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D8" s="1"/>
@@ -2681,7 +2709,7 @@
       </c>
       <c r="I12" s="38">
         <f>SUMIF(A:A,H12,E:E)</f>
-        <v>12.5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -2701,7 +2729,7 @@
       </c>
       <c r="I14" s="36">
         <f>SUMIF(A:A,H14,E:E)</f>
-        <v>0</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -2876,10 +2904,10 @@
     <mergeCell ref="H5:I5"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A50:A1048576 A18:A23 A25:A27 A30:A40 A42:A47 A5:A16 A2:A3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A50:A1048576 A18:A23 A25:A27 A30:A40 A42:A47 A2:A3 A5:A16">
       <formula1>$H$12:$H$14</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B1048576 B1:B3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B3 B5:B1048576">
       <formula1>$H$2:$H$5</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Added structure + data input and output for software
</commit_message>
<xml_diff>
--- a/Dokumentation/Aquila_Zeitaufzeichnung.xlsx
+++ b/Dokumentation/Aquila_Zeitaufzeichnung.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="3192" yWindow="0" windowWidth="20736" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="3195" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Gesamtstatus" sheetId="4" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="103">
   <si>
     <t>Arbeitspaket</t>
   </si>
@@ -300,6 +300,39 @@
   </si>
   <si>
     <t>verbessert</t>
+  </si>
+  <si>
+    <t>ASP.NET Controlls</t>
+  </si>
+  <si>
+    <t>Kenntnisse über ASP.NET</t>
+  </si>
+  <si>
+    <t>portfolio, masterpage, db</t>
+  </si>
+  <si>
+    <t>Membership Login Controller</t>
+  </si>
+  <si>
+    <t>Erkenntnisse</t>
+  </si>
+  <si>
+    <t>Chart, Portfoliodaten JSDatatables</t>
+  </si>
+  <si>
+    <t>Dynamische Tabelle 1. Chart</t>
+  </si>
+  <si>
+    <t>Masterpage eingerichtet</t>
+  </si>
+  <si>
+    <t>Web Forms, Master Pages, DB Schema</t>
+  </si>
+  <si>
+    <t>Datenbankconnectorklasse implementieren</t>
+  </si>
+  <si>
+    <t>Implementiert</t>
   </si>
 </sst>
 </file>
@@ -773,6 +806,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -860,12 +894,12 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:shape val="box"/>
-        <c:axId val="60492032"/>
-        <c:axId val="60497920"/>
+        <c:axId val="85373696"/>
+        <c:axId val="85375232"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="60492032"/>
+        <c:axId val="85373696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -874,7 +908,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60497920"/>
+        <c:crossAx val="85375232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -882,7 +916,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="60497920"/>
+        <c:axId val="85375232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -898,7 +932,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="60492032"/>
+        <c:crossAx val="85373696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -933,6 +967,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1017,13 +1052,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>20.5</c:v>
+                  <c:v>40.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.5</c:v>
+                  <c:v>17.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1039,12 +1074,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="60532608"/>
-        <c:axId val="60534144"/>
+        <c:axId val="92555904"/>
+        <c:axId val="92557696"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="60532608"/>
+        <c:axId val="92555904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1053,7 +1088,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60534144"/>
+        <c:crossAx val="92557696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1061,7 +1096,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="60534144"/>
+        <c:axId val="92557696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1072,7 +1107,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60532608"/>
+        <c:crossAx val="92555904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1443,17 +1478,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="56"/>
       <c r="B1" s="58" t="s">
         <v>24</v>
@@ -1464,7 +1499,7 @@
       <c r="D1" s="53"/>
       <c r="O1" s="11"/>
     </row>
-    <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="57"/>
       <c r="B2" s="59"/>
       <c r="C2" s="15" t="s">
@@ -1480,7 +1515,7 @@
       </c>
       <c r="B3" s="10">
         <f>SUM(B6,B12,B17)</f>
-        <v>14.5</v>
+        <v>19.5</v>
       </c>
       <c r="C3" s="28">
         <v>1</v>
@@ -1489,7 +1524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="53"/>
       <c r="B4" s="58"/>
       <c r="C4" s="60" t="s">
@@ -1497,13 +1532,13 @@
       </c>
       <c r="D4" s="61"/>
     </row>
-    <row r="5" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="57"/>
       <c r="B5" s="59"/>
       <c r="C5" s="62"/>
       <c r="D5" s="63"/>
     </row>
-    <row r="6" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>12</v>
       </c>
@@ -1518,7 +1553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>18</v>
       </c>
@@ -1529,7 +1564,7 @@
       <c r="C7" s="32"/>
       <c r="D7" s="33"/>
     </row>
-    <row r="8" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>17</v>
       </c>
@@ -1540,7 +1575,7 @@
       <c r="C8" s="32"/>
       <c r="D8" s="33"/>
     </row>
-    <row r="9" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>19</v>
       </c>
@@ -1551,7 +1586,7 @@
       <c r="C9" s="32"/>
       <c r="D9" s="33"/>
     </row>
-    <row r="10" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>20</v>
       </c>
@@ -1573,13 +1608,13 @@
       <c r="C11" s="28"/>
       <c r="D11" s="29"/>
     </row>
-    <row r="12" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="45" t="s">
         <v>65</v>
       </c>
       <c r="B12" s="19">
         <f>Software!J6</f>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C12" s="30">
         <v>1</v>
@@ -1588,7 +1623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="43" t="s">
         <v>57</v>
       </c>
@@ -1599,18 +1634,18 @@
       <c r="C13" s="32"/>
       <c r="D13" s="33"/>
     </row>
-    <row r="14" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="43" t="s">
         <v>58</v>
       </c>
       <c r="B14" s="24">
         <f>Software!J3</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C14" s="32"/>
       <c r="D14" s="33"/>
     </row>
-    <row r="15" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="43" t="s">
         <v>59</v>
       </c>
@@ -1632,7 +1667,7 @@
       <c r="C16" s="32"/>
       <c r="D16" s="33"/>
     </row>
-    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="45" t="s">
         <v>66</v>
       </c>
@@ -1647,7 +1682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="43" t="s">
         <v>61</v>
       </c>
@@ -1658,7 +1693,7 @@
       <c r="C18" s="32"/>
       <c r="D18" s="33"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="43" t="s">
         <v>62</v>
       </c>
@@ -1669,7 +1704,7 @@
       <c r="C19" s="32"/>
       <c r="D19" s="33"/>
     </row>
-    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="43" t="s">
         <v>63</v>
       </c>
@@ -1691,7 +1726,7 @@
       <c r="C21" s="28"/>
       <c r="D21" s="29"/>
     </row>
-    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="45" t="s">
         <v>67</v>
       </c>
@@ -1706,7 +1741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="43" t="s">
         <v>68</v>
       </c>
@@ -1717,7 +1752,7 @@
       <c r="C23" s="32"/>
       <c r="D23" s="33"/>
     </row>
-    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="43" t="s">
         <v>69</v>
       </c>
@@ -1739,7 +1774,7 @@
       <c r="C25" s="32"/>
       <c r="D25" s="33"/>
     </row>
-    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="45" t="s">
         <v>13</v>
       </c>
@@ -1754,7 +1789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="43" t="s">
         <v>71</v>
       </c>
@@ -1765,7 +1800,7 @@
       <c r="C27" s="32"/>
       <c r="D27" s="33"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="43" t="s">
         <v>72</v>
       </c>
@@ -1776,7 +1811,7 @@
       <c r="C28" s="32"/>
       <c r="D28" s="33"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="43" t="s">
         <v>73</v>
       </c>
@@ -1787,7 +1822,7 @@
       <c r="C29" s="32"/>
       <c r="D29" s="33"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="43" t="s">
         <v>74</v>
       </c>
@@ -1798,7 +1833,7 @@
       <c r="C30" s="32"/>
       <c r="D30" s="33"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="43" t="s">
         <v>75</v>
       </c>
@@ -1809,7 +1844,7 @@
       <c r="C31" s="32"/>
       <c r="D31" s="33"/>
     </row>
-    <row r="32" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="44" t="s">
         <v>76</v>
       </c>
@@ -1835,10 +1870,10 @@
       <c r="C35" s="55"/>
       <c r="D35" s="12">
         <f>SUM(Projektmanagement!I13,Software!I12,Website!I12,Schnittstellen!J11,'Testing &amp; Abschluss'!I13)</f>
-        <v>20.5</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+        <v>40.5</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="48" t="s">
         <v>15</v>
       </c>
@@ -1855,7 +1890,7 @@
       <c r="C37" s="51"/>
       <c r="D37" s="40">
         <f>SUM(Projektmanagement!I15,Software!I14,Website!I14,Schnittstellen!J13,'Testing &amp; Abschluss'!I15)</f>
-        <v>12.5</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1885,19 +1920,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="71.88671875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="10.88671875" style="3"/>
-    <col min="5" max="5" width="10.88671875" style="27"/>
-    <col min="6" max="6" width="24.44140625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="71.85546875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" style="3"/>
+    <col min="5" max="5" width="10.85546875" style="27"/>
+    <col min="6" max="6" width="24.42578125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1927,7 +1962,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1955,7 +1990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -1983,7 +2018,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -2011,7 +2046,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -2039,7 +2074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -2078,13 +2113,13 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D8" s="25"/>
     </row>
-    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2099,7 +2134,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D13" s="1"/>
       <c r="H13" s="35" t="s">
         <v>28</v>
@@ -2109,7 +2144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D14" s="1"/>
       <c r="H14" s="35" t="s">
         <v>6</v>
@@ -2129,15 +2164,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D16" s="1"/>
       <c r="H16" s="39"/>
       <c r="I16" s="39"/>
     </row>
-    <row r="17" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D18" s="1"/>
     </row>
   </sheetData>
@@ -2172,18 +2207,18 @@
   <dimension ref="A1:J68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="23.109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="45.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.88671875" style="3"/>
-    <col min="6" max="6" width="41.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.88671875" customWidth="1"/>
-    <col min="9" max="9" width="17.44140625" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="35.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.85546875" style="3"/>
+    <col min="6" max="6" width="41.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2213,7 +2248,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>29</v>
       </c>
@@ -2241,7 +2276,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>29</v>
       </c>
@@ -2266,10 +2301,10 @@
       <c r="I3" s="73"/>
       <c r="J3" s="4">
         <f>SUMIF(B:B,H3,E:E)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H4" s="72" t="s">
         <v>38</v>
       </c>
@@ -2298,16 +2333,33 @@
       <c r="I6" s="69"/>
       <c r="J6" s="10">
         <f>SUM(J2:J5)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="D7" s="8"/>
-    </row>
-    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D7" s="8">
+        <v>41278</v>
+      </c>
+      <c r="E7" s="3">
+        <v>5</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D9" s="7"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2322,7 +2374,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D12" s="1"/>
       <c r="H12" s="4" t="s">
         <v>28</v>
@@ -2332,7 +2384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D13" s="1"/>
       <c r="H13" s="4" t="s">
         <v>6</v>
@@ -2349,169 +2401,169 @@
       </c>
       <c r="I14" s="34">
         <f>SUMIF(A:A,H14,E:E)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D32" s="1"/>
     </row>
-    <row r="33" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D33" s="1"/>
     </row>
-    <row r="34" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D34" s="1"/>
     </row>
-    <row r="35" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D35" s="1"/>
     </row>
-    <row r="36" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D36" s="1"/>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D37" s="1"/>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D38" s="1"/>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D40" s="1"/>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D41" s="1"/>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D42" s="1"/>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D43" s="1"/>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D44" s="1"/>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D45" s="1"/>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D46" s="1"/>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D47" s="1"/>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D48" s="1"/>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D49" s="1"/>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D50" s="1"/>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D51" s="1"/>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D52" s="1"/>
     </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D53" s="1"/>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D54" s="1"/>
     </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D55" s="1"/>
     </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D56" s="1"/>
     </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D57" s="1"/>
     </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D58" s="1"/>
     </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D59" s="1"/>
     </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D60" s="1"/>
     </row>
-    <row r="61" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D61" s="1"/>
     </row>
-    <row r="62" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D62" s="1"/>
     </row>
-    <row r="63" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D63" s="1"/>
     </row>
-    <row r="64" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D64" s="1"/>
     </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D65" s="1"/>
     </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D66" s="1"/>
     </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D67" s="1"/>
     </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D68" s="1"/>
     </row>
   </sheetData>
@@ -2545,19 +2597,19 @@
   <dimension ref="A1:J68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" style="3" customWidth="1"/>
     <col min="2" max="2" width="30" style="3" customWidth="1"/>
-    <col min="3" max="3" width="45.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.88671875" style="3"/>
-    <col min="5" max="5" width="10.88671875" style="47"/>
-    <col min="6" max="6" width="41.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.88671875" customWidth="1"/>
-    <col min="9" max="9" width="17.44140625" customWidth="1"/>
+    <col min="3" max="3" width="45.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" style="3"/>
+    <col min="5" max="5" width="10.85546875" style="47"/>
+    <col min="6" max="6" width="41.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2587,7 +2639,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>28</v>
       </c>
@@ -2615,7 +2667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>28</v>
       </c>
@@ -2643,7 +2695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>28</v>
       </c>
@@ -2671,7 +2723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>28</v>
       </c>
@@ -2699,7 +2751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>28</v>
       </c>
@@ -2724,7 +2776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>29</v>
       </c>
@@ -2741,7 +2793,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>28</v>
       </c>
@@ -2758,7 +2810,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>28</v>
       </c>
@@ -2798,7 +2850,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>29</v>
       </c>
@@ -2824,18 +2876,52 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="D12" s="1"/>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D12" s="1">
+        <v>41270</v>
+      </c>
+      <c r="E12" s="47">
+        <v>2</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="H12" s="38" t="s">
         <v>28</v>
       </c>
       <c r="I12" s="38">
         <f>SUMIF(A:A,H12,E:E)</f>
-        <v>20.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="D13" s="1"/>
+        <v>40.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13" s="1">
+        <v>41271</v>
+      </c>
+      <c r="E13" s="47">
+        <v>4</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>96</v>
+      </c>
       <c r="H13" s="38" t="s">
         <v>6</v>
       </c>
@@ -2845,7 +2931,24 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="1"/>
+      <c r="A14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D14" s="1">
+        <v>41274</v>
+      </c>
+      <c r="E14" s="47">
+        <v>3</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>96</v>
+      </c>
       <c r="H14" s="36" t="s">
         <v>29</v>
       </c>
@@ -2854,166 +2957,200 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D15" s="1">
+        <v>40912</v>
+      </c>
+      <c r="E15" s="47">
+        <v>8</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D16" s="1">
+        <v>40913</v>
+      </c>
+      <c r="E16" s="47">
+        <v>3</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D32" s="1"/>
     </row>
-    <row r="33" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D33" s="1"/>
     </row>
-    <row r="34" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D34" s="1"/>
     </row>
-    <row r="35" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D35" s="1"/>
     </row>
-    <row r="36" spans="4:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D36" s="1"/>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D37" s="1"/>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D38" s="1"/>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D40" s="1"/>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D41" s="1"/>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D42" s="1"/>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D43" s="1"/>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D44" s="1"/>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D45" s="1"/>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D46" s="1"/>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D47" s="1"/>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D48" s="1"/>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D49" s="1"/>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D50" s="1"/>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D51" s="1"/>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D52" s="1"/>
     </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D53" s="1"/>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D54" s="1"/>
     </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D55" s="1"/>
     </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D56" s="1"/>
     </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D57" s="1"/>
     </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D58" s="1"/>
     </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D59" s="1"/>
     </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D60" s="1"/>
     </row>
-    <row r="61" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D61" s="1"/>
     </row>
-    <row r="62" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D62" s="1"/>
     </row>
-    <row r="63" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D63" s="1"/>
     </row>
-    <row r="64" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D64" s="1"/>
     </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D65" s="1"/>
     </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D66" s="1"/>
     </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D67" s="1"/>
     </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D68" s="1"/>
     </row>
   </sheetData>
@@ -3026,7 +3163,7 @@
     <mergeCell ref="H5:I5"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A50:A1048576 A18:A23 A25:A27 A30:A40 A42:A47 A2:A3 A5:A16">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A50:A1048576 A25:A27 A30:A40 A42:A47 A2:A3 A5:A23">
       <formula1>$H$12:$H$14</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B3 B5:B1048576">
@@ -3051,16 +3188,16 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" style="3" customWidth="1"/>
     <col min="2" max="2" width="39" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.88671875" style="3"/>
-    <col min="6" max="6" width="41.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.88671875" customWidth="1"/>
-    <col min="8" max="8" width="20.6640625" customWidth="1"/>
-    <col min="9" max="9" width="21.88671875" customWidth="1"/>
+    <col min="3" max="3" width="45.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.85546875" style="3"/>
+    <col min="6" max="6" width="41.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.85546875" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3090,7 +3227,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -3110,7 +3247,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D3" s="7"/>
       <c r="H3" s="68" t="s">
         <v>45</v>
@@ -3143,13 +3280,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D6" s="8"/>
     </row>
-    <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D8" s="7"/>
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3164,7 +3301,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D11" s="1"/>
       <c r="H11" s="42" t="s">
         <v>28</v>
@@ -3174,7 +3311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D12" s="1"/>
       <c r="H12" s="42" t="s">
         <v>6</v>
@@ -3194,370 +3331,370 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D16" s="1"/>
       <c r="G16"/>
       <c r="H16"/>
       <c r="I16"/>
       <c r="J16"/>
     </row>
-    <row r="17" spans="4:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D17" s="1"/>
       <c r="G17"/>
       <c r="H17"/>
       <c r="I17"/>
       <c r="J17"/>
     </row>
-    <row r="18" spans="4:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D18" s="1"/>
       <c r="G18"/>
       <c r="H18"/>
       <c r="I18"/>
       <c r="J18"/>
     </row>
-    <row r="19" spans="4:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D19" s="1"/>
       <c r="G19"/>
       <c r="H19"/>
       <c r="I19"/>
       <c r="J19"/>
     </row>
-    <row r="20" spans="4:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D20" s="1"/>
       <c r="G20"/>
       <c r="H20"/>
       <c r="I20"/>
       <c r="J20"/>
     </row>
-    <row r="21" spans="4:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D21" s="1"/>
       <c r="G21"/>
       <c r="H21"/>
       <c r="I21"/>
       <c r="J21"/>
     </row>
-    <row r="22" spans="4:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D22" s="1"/>
       <c r="G22"/>
       <c r="H22"/>
       <c r="I22"/>
       <c r="J22"/>
     </row>
-    <row r="23" spans="4:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D23" s="1"/>
       <c r="G23"/>
       <c r="H23"/>
       <c r="I23"/>
       <c r="J23"/>
     </row>
-    <row r="24" spans="4:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D24" s="1"/>
       <c r="G24"/>
       <c r="H24"/>
       <c r="I24"/>
       <c r="J24"/>
     </row>
-    <row r="25" spans="4:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D25" s="1"/>
       <c r="G25"/>
       <c r="H25"/>
       <c r="I25"/>
       <c r="J25"/>
     </row>
-    <row r="26" spans="4:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D26" s="1"/>
       <c r="G26"/>
       <c r="H26"/>
       <c r="I26"/>
       <c r="J26"/>
     </row>
-    <row r="27" spans="4:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D27" s="1"/>
       <c r="G27"/>
       <c r="H27"/>
       <c r="I27"/>
       <c r="J27"/>
     </row>
-    <row r="28" spans="4:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D28" s="1"/>
       <c r="G28"/>
       <c r="H28"/>
       <c r="I28"/>
       <c r="J28"/>
     </row>
-    <row r="29" spans="4:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D29" s="1"/>
       <c r="G29"/>
       <c r="H29"/>
       <c r="I29"/>
       <c r="J29"/>
     </row>
-    <row r="30" spans="4:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D30" s="1"/>
       <c r="G30"/>
       <c r="H30"/>
       <c r="I30"/>
       <c r="J30"/>
     </row>
-    <row r="31" spans="4:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D31" s="1"/>
       <c r="G31"/>
       <c r="H31"/>
       <c r="I31"/>
       <c r="J31"/>
     </row>
-    <row r="32" spans="4:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D32" s="1"/>
       <c r="G32"/>
       <c r="H32"/>
       <c r="I32"/>
       <c r="J32"/>
     </row>
-    <row r="33" spans="4:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D33" s="1"/>
       <c r="G33"/>
       <c r="H33"/>
       <c r="I33"/>
       <c r="J33"/>
     </row>
-    <row r="34" spans="4:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D34" s="1"/>
       <c r="G34"/>
       <c r="H34"/>
       <c r="I34"/>
       <c r="J34"/>
     </row>
-    <row r="35" spans="4:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D35" s="1"/>
       <c r="G35"/>
       <c r="H35"/>
       <c r="I35"/>
       <c r="J35"/>
     </row>
-    <row r="36" spans="4:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D36" s="1"/>
       <c r="G36"/>
       <c r="H36"/>
       <c r="I36"/>
       <c r="J36"/>
     </row>
-    <row r="37" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D37" s="1"/>
       <c r="G37"/>
       <c r="H37"/>
       <c r="I37"/>
       <c r="J37"/>
     </row>
-    <row r="38" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D38" s="1"/>
       <c r="G38"/>
       <c r="H38"/>
       <c r="I38"/>
       <c r="J38"/>
     </row>
-    <row r="39" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D39" s="1"/>
       <c r="G39"/>
       <c r="H39"/>
       <c r="I39"/>
       <c r="J39"/>
     </row>
-    <row r="40" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D40" s="1"/>
       <c r="G40"/>
       <c r="H40"/>
       <c r="I40"/>
       <c r="J40"/>
     </row>
-    <row r="41" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D41" s="1"/>
       <c r="G41"/>
       <c r="H41"/>
       <c r="I41"/>
       <c r="J41"/>
     </row>
-    <row r="42" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D42" s="1"/>
       <c r="G42"/>
       <c r="H42"/>
       <c r="I42"/>
       <c r="J42"/>
     </row>
-    <row r="43" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D43" s="1"/>
       <c r="G43"/>
       <c r="H43"/>
       <c r="I43"/>
       <c r="J43"/>
     </row>
-    <row r="44" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D44" s="1"/>
       <c r="G44"/>
       <c r="H44"/>
       <c r="I44"/>
       <c r="J44"/>
     </row>
-    <row r="45" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D45" s="1"/>
       <c r="G45"/>
       <c r="H45"/>
       <c r="I45"/>
       <c r="J45"/>
     </row>
-    <row r="46" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D46" s="1"/>
       <c r="G46"/>
       <c r="H46"/>
       <c r="I46"/>
       <c r="J46"/>
     </row>
-    <row r="47" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D47" s="1"/>
       <c r="G47"/>
       <c r="H47"/>
       <c r="I47"/>
       <c r="J47"/>
     </row>
-    <row r="48" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D48" s="1"/>
       <c r="G48"/>
       <c r="H48"/>
       <c r="I48"/>
       <c r="J48"/>
     </row>
-    <row r="49" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D49" s="1"/>
       <c r="G49"/>
       <c r="H49"/>
       <c r="I49"/>
       <c r="J49"/>
     </row>
-    <row r="50" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D50" s="1"/>
       <c r="G50"/>
       <c r="H50"/>
       <c r="I50"/>
       <c r="J50"/>
     </row>
-    <row r="51" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D51" s="1"/>
       <c r="G51"/>
       <c r="H51"/>
       <c r="I51"/>
       <c r="J51"/>
     </row>
-    <row r="52" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D52" s="1"/>
       <c r="G52"/>
       <c r="H52"/>
       <c r="I52"/>
       <c r="J52"/>
     </row>
-    <row r="53" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D53" s="1"/>
       <c r="G53"/>
       <c r="H53"/>
       <c r="I53"/>
       <c r="J53"/>
     </row>
-    <row r="54" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D54" s="1"/>
       <c r="G54"/>
       <c r="H54"/>
       <c r="I54"/>
       <c r="J54"/>
     </row>
-    <row r="55" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D55" s="1"/>
       <c r="G55"/>
       <c r="H55"/>
       <c r="I55"/>
       <c r="J55"/>
     </row>
-    <row r="56" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D56" s="1"/>
       <c r="G56"/>
       <c r="H56"/>
       <c r="I56"/>
       <c r="J56"/>
     </row>
-    <row r="57" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D57" s="1"/>
       <c r="G57"/>
       <c r="H57"/>
       <c r="I57"/>
       <c r="J57"/>
     </row>
-    <row r="58" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D58" s="1"/>
       <c r="G58"/>
       <c r="H58"/>
       <c r="I58"/>
       <c r="J58"/>
     </row>
-    <row r="59" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D59" s="1"/>
       <c r="G59"/>
       <c r="H59"/>
       <c r="I59"/>
       <c r="J59"/>
     </row>
-    <row r="60" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D60" s="1"/>
       <c r="G60"/>
       <c r="H60"/>
       <c r="I60"/>
       <c r="J60"/>
     </row>
-    <row r="61" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D61" s="1"/>
       <c r="G61"/>
       <c r="H61"/>
       <c r="I61"/>
       <c r="J61"/>
     </row>
-    <row r="62" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D62" s="1"/>
       <c r="G62"/>
       <c r="H62"/>
       <c r="I62"/>
       <c r="J62"/>
     </row>
-    <row r="63" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D63" s="1"/>
       <c r="G63"/>
       <c r="H63"/>
       <c r="I63"/>
       <c r="J63"/>
     </row>
-    <row r="64" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D64" s="1"/>
       <c r="G64"/>
       <c r="H64"/>
       <c r="I64"/>
       <c r="J64"/>
     </row>
-    <row r="65" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D65" s="1"/>
       <c r="G65"/>
       <c r="H65"/>
       <c r="I65"/>
       <c r="J65"/>
     </row>
-    <row r="66" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D66" s="1"/>
       <c r="G66"/>
       <c r="H66"/>
       <c r="I66"/>
       <c r="J66"/>
     </row>
-    <row r="67" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D67" s="1"/>
       <c r="G67"/>
       <c r="H67"/>
@@ -3597,16 +3734,16 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" style="3" customWidth="1"/>
-    <col min="3" max="3" width="86.6640625" style="3" customWidth="1"/>
-    <col min="4" max="5" width="10.88671875" style="3"/>
-    <col min="6" max="6" width="45.88671875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="7.109375" customWidth="1"/>
-    <col min="8" max="8" width="15.109375" customWidth="1"/>
-    <col min="9" max="9" width="16.109375" customWidth="1"/>
+    <col min="3" max="3" width="86.7109375" style="3" customWidth="1"/>
+    <col min="4" max="5" width="10.85546875" style="3"/>
+    <col min="6" max="6" width="45.85546875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="7.140625" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3636,7 +3773,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D2" s="1"/>
       <c r="H2" s="70" t="s">
         <v>47</v>
@@ -3647,7 +3784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D3" s="1"/>
       <c r="H3" s="68" t="s">
         <v>48</v>
@@ -3658,7 +3795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D4" s="1"/>
       <c r="H4" s="68" t="s">
         <v>49</v>
@@ -3669,7 +3806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D5" s="1"/>
       <c r="H5" s="68" t="s">
         <v>50</v>
@@ -3680,7 +3817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D6" s="1"/>
       <c r="H6" s="72" t="s">
         <v>51</v>
@@ -3691,7 +3828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D7" s="1"/>
       <c r="H7" s="74" t="s">
         <v>52</v>
@@ -3713,10 +3850,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3730,7 +3867,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H13" s="35" t="s">
         <v>28</v>
       </c>
@@ -3739,7 +3876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H14" s="35" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Updated Projektstatusbericht & Aquila_Zeitaufzeichnung
</commit_message>
<xml_diff>
--- a/Dokumentation/Aquila_Zeitaufzeichnung.xlsx
+++ b/Dokumentation/Aquila_Zeitaufzeichnung.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="0" windowWidth="20740" windowHeight="11760" activeTab="3"/>
+    <workbookView xWindow="3204" yWindow="0" windowWidth="20736" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Gesamtstatus" sheetId="4" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <sheet name="Schnittstellen" sheetId="7" r:id="rId5"/>
     <sheet name="Testing &amp; Abschluss" sheetId="3" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="127">
   <si>
     <t>Arbeitspaket</t>
   </si>
@@ -387,6 +387,24 @@
   </si>
   <si>
     <t>Interaktives Hinzufügen</t>
+  </si>
+  <si>
+    <t>Aufbau der Grundstruktur der Software</t>
+  </si>
+  <si>
+    <t>Grundstruktur fertiggestellt</t>
+  </si>
+  <si>
+    <t>Broker-Schnittstelle 50%</t>
+  </si>
+  <si>
+    <t>Daten-Schnittstellen-Prototyp implementiert</t>
+  </si>
+  <si>
+    <t>Kauf-/Verkaufschnittstelle 50%</t>
+  </si>
+  <si>
+    <t>Kauf-/Verkaufschnittstellen-Prototyp implementiert</t>
   </si>
 </sst>
 </file>
@@ -809,14 +827,14 @@
     </xf>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -837,7 +855,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="de-AT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -933,10 +951,10 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -952,12 +970,12 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:shape val="box"/>
-        <c:axId val="2074863416"/>
-        <c:axId val="2074859400"/>
+        <c:axId val="34432896"/>
+        <c:axId val="34434432"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="2074863416"/>
+        <c:axId val="34432896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -966,7 +984,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2074859400"/>
+        <c:crossAx val="34434432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -974,7 +992,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2074859400"/>
+        <c:axId val="34434432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -990,7 +1008,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2074863416"/>
+        <c:crossAx val="34432896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1004,7 +1022,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.787401575" l="0.7" r="0.7" t="0.787401575" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1013,7 +1031,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="de-AT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1081,7 +1099,6 @@
                 <a:schemeClr val="tx2">
                   <a:lumMod val="60000"/>
                   <a:lumOff val="40000"/>
-                  <a:alpha val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
             </c:spPr>
@@ -1110,10 +1127,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>66.0</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.5</c:v>
+                  <c:v>14.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>23.5</c:v>
@@ -1132,12 +1149,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="2074936392"/>
-        <c:axId val="2074939368"/>
+        <c:axId val="34467840"/>
+        <c:axId val="34469376"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="2074936392"/>
+        <c:axId val="34467840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1146,7 +1163,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2074939368"/>
+        <c:crossAx val="34469376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1154,7 +1171,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2074939368"/>
+        <c:axId val="34469376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1165,7 +1182,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2074936392"/>
+        <c:crossAx val="34467840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1176,7 +1193,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.787401575" l="0.7" r="0.7" t="0.787401575" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1536,17 +1553,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="45" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="56"/>
       <c r="B1" s="58" t="s">
         <v>24</v>
@@ -1557,7 +1574,7 @@
       <c r="D1" s="53"/>
       <c r="O1" s="11"/>
     </row>
-    <row r="2" spans="1:15" ht="15" thickBot="1">
+    <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="57"/>
       <c r="B2" s="59"/>
       <c r="C2" s="15" t="s">
@@ -1567,13 +1584,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15" thickBot="1">
+    <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="10">
         <f>SUM(B6,B12,B17)</f>
-        <v>21.5</v>
+        <v>30.5</v>
       </c>
       <c r="C3" s="28">
         <v>1</v>
@@ -1582,7 +1599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="53"/>
       <c r="B4" s="58"/>
       <c r="C4" s="60" t="s">
@@ -1590,13 +1607,13 @@
       </c>
       <c r="D4" s="61"/>
     </row>
-    <row r="5" spans="1:15" ht="15" thickBot="1">
+    <row r="5" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="57"/>
       <c r="B5" s="59"/>
       <c r="C5" s="62"/>
       <c r="D5" s="63"/>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>12</v>
       </c>
@@ -1611,7 +1628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>18</v>
       </c>
@@ -1622,7 +1639,7 @@
       <c r="C7" s="32"/>
       <c r="D7" s="33"/>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
         <v>17</v>
       </c>
@@ -1633,7 +1650,7 @@
       <c r="C8" s="32"/>
       <c r="D8" s="33"/>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>19</v>
       </c>
@@ -1644,7 +1661,7 @@
       <c r="C9" s="32"/>
       <c r="D9" s="33"/>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>20</v>
       </c>
@@ -1655,7 +1672,7 @@
       <c r="C10" s="32"/>
       <c r="D10" s="33"/>
     </row>
-    <row r="11" spans="1:15" ht="15" thickBot="1">
+    <row r="11" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="22" t="s">
         <v>21</v>
       </c>
@@ -1666,13 +1683,13 @@
       <c r="C11" s="28"/>
       <c r="D11" s="29"/>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="45" t="s">
         <v>65</v>
       </c>
       <c r="B12" s="19">
         <f>Software!J6</f>
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="C12" s="30">
         <v>1</v>
@@ -1681,18 +1698,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="43" t="s">
         <v>57</v>
       </c>
       <c r="B13" s="24">
         <f>Software!J2</f>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C13" s="32"/>
       <c r="D13" s="33"/>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="43" t="s">
         <v>58</v>
       </c>
@@ -1703,18 +1720,18 @@
       <c r="C14" s="32"/>
       <c r="D14" s="33"/>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="43" t="s">
         <v>59</v>
       </c>
       <c r="B15" s="24">
         <f>Software!J4</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C15" s="32"/>
       <c r="D15" s="33"/>
     </row>
-    <row r="16" spans="1:15" ht="15" thickBot="1">
+    <row r="16" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="43" t="s">
         <v>60</v>
       </c>
@@ -1725,7 +1742,7 @@
       <c r="C16" s="32"/>
       <c r="D16" s="33"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="45" t="s">
         <v>66</v>
       </c>
@@ -1740,7 +1757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="43" t="s">
         <v>61</v>
       </c>
@@ -1751,7 +1768,7 @@
       <c r="C18" s="32"/>
       <c r="D18" s="33"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="43" t="s">
         <v>62</v>
       </c>
@@ -1762,7 +1779,7 @@
       <c r="C19" s="32"/>
       <c r="D19" s="33"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="43" t="s">
         <v>63</v>
       </c>
@@ -1773,7 +1790,7 @@
       <c r="C20" s="32"/>
       <c r="D20" s="33"/>
     </row>
-    <row r="21" spans="1:4" ht="15" thickBot="1">
+    <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="44" t="s">
         <v>64</v>
       </c>
@@ -1784,7 +1801,7 @@
       <c r="C21" s="28"/>
       <c r="D21" s="29"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="45" t="s">
         <v>67</v>
       </c>
@@ -1799,7 +1816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="43" t="s">
         <v>68</v>
       </c>
@@ -1810,7 +1827,7 @@
       <c r="C23" s="32"/>
       <c r="D23" s="33"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="43" t="s">
         <v>69</v>
       </c>
@@ -1821,7 +1838,7 @@
       <c r="C24" s="32"/>
       <c r="D24" s="33"/>
     </row>
-    <row r="25" spans="1:4" ht="15" thickBot="1">
+    <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="43" t="s">
         <v>70</v>
       </c>
@@ -1832,7 +1849,7 @@
       <c r="C25" s="32"/>
       <c r="D25" s="33"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="45" t="s">
         <v>13</v>
       </c>
@@ -1847,7 +1864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="43" t="s">
         <v>71</v>
       </c>
@@ -1858,7 +1875,7 @@
       <c r="C27" s="32"/>
       <c r="D27" s="33"/>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="43" t="s">
         <v>72</v>
       </c>
@@ -1869,7 +1886,7 @@
       <c r="C28" s="32"/>
       <c r="D28" s="33"/>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="43" t="s">
         <v>73</v>
       </c>
@@ -1880,7 +1897,7 @@
       <c r="C29" s="32"/>
       <c r="D29" s="33"/>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="43" t="s">
         <v>74</v>
       </c>
@@ -1891,7 +1908,7 @@
       <c r="C30" s="32"/>
       <c r="D30" s="33"/>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="43" t="s">
         <v>75</v>
       </c>
@@ -1902,7 +1919,7 @@
       <c r="C31" s="32"/>
       <c r="D31" s="33"/>
     </row>
-    <row r="32" spans="1:4" ht="15" thickBot="1">
+    <row r="32" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="44" t="s">
         <v>76</v>
       </c>
@@ -1913,15 +1930,15 @@
       <c r="C32" s="46"/>
       <c r="D32" s="29"/>
     </row>
-    <row r="33" spans="2:4" ht="15" thickBot="1"/>
-    <row r="34" spans="2:4" ht="15" thickBot="1">
+    <row r="33" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="34" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B34" s="13"/>
       <c r="C34" s="14" t="s">
         <v>27</v>
       </c>
       <c r="D34" s="41"/>
     </row>
-    <row r="35" spans="2:4" ht="15" customHeight="1">
+    <row r="35" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="54" t="s">
         <v>30</v>
       </c>
@@ -1931,17 +1948,17 @@
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="2:4">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B36" s="48" t="s">
         <v>15</v>
       </c>
       <c r="C36" s="49"/>
       <c r="D36" s="42">
         <f>SUM(Projektmanagement!I14,Software!I13,Website!I13,Schnittstellen!J12,'Testing &amp; Abschluss'!I14)</f>
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" ht="15" thickBot="1">
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B37" s="50" t="s">
         <v>31</v>
       </c>
@@ -1951,7 +1968,7 @@
         <v>23.5</v>
       </c>
     </row>
-    <row r="38" spans="2:4" ht="15.75" customHeight="1"/>
+    <row r="38" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="B36:C36"/>
@@ -1982,18 +1999,18 @@
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.77734375" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.33203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="71.83203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="3"/>
-    <col min="5" max="5" width="10.83203125" style="27"/>
-    <col min="6" max="6" width="24.5" style="3" customWidth="1"/>
-    <col min="9" max="9" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="71.77734375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="10.77734375" style="3"/>
+    <col min="5" max="5" width="10.77734375" style="27"/>
+    <col min="6" max="6" width="24.44140625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="12.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1">
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>32</v>
       </c>
@@ -2020,7 +2037,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2048,7 +2065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -2076,7 +2093,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -2104,7 +2121,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -2132,7 +2149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1">
+    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -2160,7 +2177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15" thickBot="1">
+    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D7" s="1"/>
       <c r="H7" s="64" t="s">
         <v>16</v>
@@ -2171,19 +2188,19 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D8" s="25"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:10" ht="15" thickBot="1">
+    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:10" ht="15" thickBot="1">
+    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D12" s="1"/>
       <c r="H12" s="6" t="s">
         <v>5</v>
@@ -2192,7 +2209,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D13" s="1"/>
       <c r="H13" s="35" t="s">
         <v>28</v>
@@ -2202,7 +2219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D14" s="1"/>
       <c r="H14" s="35" t="s">
         <v>6</v>
@@ -2212,7 +2229,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1">
+    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D15" s="1"/>
       <c r="H15" s="35" t="s">
         <v>29</v>
@@ -2222,15 +2239,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D16" s="1"/>
       <c r="H16" s="39"/>
       <c r="I16" s="39"/>
     </row>
-    <row r="17" spans="4:4">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="4:4">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D18" s="1"/>
     </row>
   </sheetData>
@@ -2265,21 +2282,21 @@
   <dimension ref="A1:J68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.33203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="35.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.83203125" style="3"/>
+    <col min="2" max="2" width="31.44140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="45.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.77734375" style="3"/>
     <col min="6" max="6" width="41.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.83203125" customWidth="1"/>
-    <col min="9" max="9" width="17.5" customWidth="1"/>
+    <col min="8" max="8" width="15.77734375" customWidth="1"/>
+    <col min="9" max="9" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1">
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
@@ -2306,7 +2323,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>29</v>
       </c>
@@ -2331,10 +2348,10 @@
       <c r="I2" s="71"/>
       <c r="J2" s="4">
         <f>SUMIF(B:B,H2,E:E)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>29</v>
       </c>
@@ -2362,18 +2379,53 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D4" s="9">
+        <v>41269</v>
+      </c>
+      <c r="E4" s="3">
+        <v>3</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>122</v>
+      </c>
       <c r="H4" s="72" t="s">
         <v>38</v>
       </c>
       <c r="I4" s="73"/>
       <c r="J4" s="4">
         <f>SUMIF(B:B,H4,E:E)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="15" thickBot="1">
-      <c r="D5" s="9"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D5" s="9">
+        <v>41271</v>
+      </c>
+      <c r="E5" s="3">
+        <v>3</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>123</v>
+      </c>
       <c r="H5" s="74" t="s">
         <v>39</v>
       </c>
@@ -2383,18 +2435,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1">
-      <c r="D6" s="1"/>
+    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D6" s="1">
+        <v>41276</v>
+      </c>
+      <c r="E6" s="3">
+        <v>3</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>125</v>
+      </c>
       <c r="H6" s="64" t="s">
         <v>16</v>
       </c>
       <c r="I6" s="69"/>
       <c r="J6" s="10">
         <f>SUM(J2:J5)</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>29</v>
       </c>
@@ -2414,7 +2483,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>29</v>
       </c>
@@ -2434,13 +2503,13 @@
         <v>111</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:10" ht="15" thickBot="1">
+    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:10" ht="15" thickBot="1">
+    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D11" s="1"/>
       <c r="H11" s="6" t="s">
         <v>5</v>
@@ -2449,7 +2518,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D12" s="1"/>
       <c r="H12" s="4" t="s">
         <v>28</v>
@@ -2459,17 +2528,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D13" s="1"/>
       <c r="H13" s="4" t="s">
         <v>6</v>
       </c>
       <c r="I13" s="4">
         <f>SUMIF(A:A,H13,E:E)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="15" thickBot="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D14" s="1"/>
       <c r="H14" s="34" t="s">
         <v>29</v>
@@ -2479,166 +2548,166 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="4:4">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="4:4">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="4:4">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="4:4">
+    <row r="20" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="4:4">
+    <row r="21" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="4:4">
+    <row r="22" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="4:4">
+    <row r="23" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="4:4">
+    <row r="24" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="4:4">
+    <row r="25" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="4:4">
+    <row r="26" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="4:4">
+    <row r="27" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="4:4">
+    <row r="28" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="4:4">
+    <row r="29" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="4:4">
+    <row r="30" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="4:4">
+    <row r="31" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="4:4">
+    <row r="32" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D32" s="1"/>
     </row>
-    <row r="33" spans="4:4">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D33" s="1"/>
     </row>
-    <row r="34" spans="4:4">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D34" s="1"/>
     </row>
-    <row r="35" spans="4:4">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D35" s="1"/>
     </row>
-    <row r="36" spans="4:4">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D36" s="1"/>
     </row>
-    <row r="37" spans="4:4">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D37" s="1"/>
     </row>
-    <row r="38" spans="4:4">
+    <row r="38" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D38" s="1"/>
     </row>
-    <row r="39" spans="4:4">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="4:4">
+    <row r="40" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D40" s="1"/>
     </row>
-    <row r="41" spans="4:4">
+    <row r="41" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D41" s="1"/>
     </row>
-    <row r="42" spans="4:4">
+    <row r="42" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D42" s="1"/>
     </row>
-    <row r="43" spans="4:4">
+    <row r="43" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D43" s="1"/>
     </row>
-    <row r="44" spans="4:4">
+    <row r="44" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D44" s="1"/>
     </row>
-    <row r="45" spans="4:4">
+    <row r="45" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D45" s="1"/>
     </row>
-    <row r="46" spans="4:4">
+    <row r="46" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D46" s="1"/>
     </row>
-    <row r="47" spans="4:4">
+    <row r="47" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D47" s="1"/>
     </row>
-    <row r="48" spans="4:4">
+    <row r="48" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D48" s="1"/>
     </row>
-    <row r="49" spans="4:4">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D49" s="1"/>
     </row>
-    <row r="50" spans="4:4">
+    <row r="50" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D50" s="1"/>
     </row>
-    <row r="51" spans="4:4">
+    <row r="51" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D51" s="1"/>
     </row>
-    <row r="52" spans="4:4">
+    <row r="52" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D52" s="1"/>
     </row>
-    <row r="53" spans="4:4">
+    <row r="53" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D53" s="1"/>
     </row>
-    <row r="54" spans="4:4">
+    <row r="54" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D54" s="1"/>
     </row>
-    <row r="55" spans="4:4">
+    <row r="55" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D55" s="1"/>
     </row>
-    <row r="56" spans="4:4">
+    <row r="56" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D56" s="1"/>
     </row>
-    <row r="57" spans="4:4">
+    <row r="57" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D57" s="1"/>
     </row>
-    <row r="58" spans="4:4">
+    <row r="58" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D58" s="1"/>
     </row>
-    <row r="59" spans="4:4">
+    <row r="59" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D59" s="1"/>
     </row>
-    <row r="60" spans="4:4">
+    <row r="60" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D60" s="1"/>
     </row>
-    <row r="61" spans="4:4">
+    <row r="61" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D61" s="1"/>
     </row>
-    <row r="62" spans="4:4">
+    <row r="62" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D62" s="1"/>
     </row>
-    <row r="63" spans="4:4">
+    <row r="63" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D63" s="1"/>
     </row>
-    <row r="64" spans="4:4">
+    <row r="64" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D64" s="1"/>
     </row>
-    <row r="65" spans="4:4">
+    <row r="65" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D65" s="1"/>
     </row>
-    <row r="66" spans="4:4">
+    <row r="66" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D66" s="1"/>
     </row>
-    <row r="67" spans="4:4">
+    <row r="67" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D67" s="1"/>
     </row>
-    <row r="68" spans="4:4">
+    <row r="68" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D68" s="1"/>
     </row>
   </sheetData>
@@ -2651,7 +2720,7 @@
     <mergeCell ref="H5:I5"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A50:A1048576 A18:A23 A25:A27 A30:A40 A42:A47 A2:A3 A5:A16">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A50:A1048576 A18:A23 A25:A27 A30:A40 A42:A47 A2:A16">
       <formula1>$H$12:$H$14</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17:B23 B49:B1048576 B41:B46 B29:B39 B25:B27 B1:B15">
@@ -2671,23 +2740,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.33203125" style="3" customWidth="1"/>
     <col min="2" max="2" width="30" style="3" customWidth="1"/>
-    <col min="3" max="3" width="45.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="3"/>
-    <col min="5" max="5" width="10.83203125" style="47"/>
+    <col min="3" max="3" width="45.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.77734375" style="3"/>
+    <col min="5" max="5" width="10.77734375" style="47"/>
     <col min="6" max="6" width="41.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.83203125" customWidth="1"/>
-    <col min="9" max="9" width="17.5" customWidth="1"/>
+    <col min="8" max="8" width="15.77734375" customWidth="1"/>
+    <col min="9" max="9" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1">
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
@@ -2714,7 +2783,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>28</v>
       </c>
@@ -2742,7 +2811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>28</v>
       </c>
@@ -2770,7 +2839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>28</v>
       </c>
@@ -2798,7 +2867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15" thickBot="1">
+    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>28</v>
       </c>
@@ -2826,7 +2895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1">
+    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>28</v>
       </c>
@@ -2851,7 +2920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>29</v>
       </c>
@@ -2868,7 +2937,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>28</v>
       </c>
@@ -2885,7 +2954,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>28</v>
       </c>
@@ -2905,7 +2974,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15" thickBot="1">
+    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>28</v>
       </c>
@@ -2925,7 +2994,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15" thickBot="1">
+    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>29</v>
       </c>
@@ -2951,7 +3020,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>28</v>
       </c>
@@ -2978,7 +3047,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>28</v>
       </c>
@@ -3005,7 +3074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15" thickBot="1">
+    <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>28</v>
       </c>
@@ -3032,7 +3101,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>28</v>
       </c>
@@ -3052,7 +3121,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>28</v>
       </c>
@@ -3072,7 +3141,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>28</v>
       </c>
@@ -3092,7 +3161,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>28</v>
       </c>
@@ -3112,7 +3181,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>29</v>
       </c>
@@ -3132,7 +3201,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>28</v>
       </c>
@@ -3152,7 +3221,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>28</v>
       </c>
@@ -3172,7 +3241,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>28</v>
       </c>
@@ -3192,7 +3261,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>28</v>
       </c>
@@ -3212,7 +3281,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>28</v>
       </c>
@@ -3223,136 +3292,136 @@
         <v>41303</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D32" s="1"/>
     </row>
-    <row r="33" spans="4:4">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D33" s="1"/>
     </row>
-    <row r="34" spans="4:4">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D34" s="1"/>
     </row>
-    <row r="35" spans="4:4">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D35" s="1"/>
     </row>
-    <row r="36" spans="4:4">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D36" s="1"/>
     </row>
-    <row r="37" spans="4:4">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D37" s="1"/>
     </row>
-    <row r="38" spans="4:4">
+    <row r="38" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D38" s="1"/>
     </row>
-    <row r="39" spans="4:4">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="4:4">
+    <row r="40" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D40" s="1"/>
     </row>
-    <row r="41" spans="4:4">
+    <row r="41" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D41" s="1"/>
     </row>
-    <row r="42" spans="4:4">
+    <row r="42" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D42" s="1"/>
     </row>
-    <row r="43" spans="4:4">
+    <row r="43" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D43" s="1"/>
     </row>
-    <row r="44" spans="4:4">
+    <row r="44" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D44" s="1"/>
     </row>
-    <row r="45" spans="4:4">
+    <row r="45" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D45" s="1"/>
     </row>
-    <row r="46" spans="4:4">
+    <row r="46" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D46" s="1"/>
     </row>
-    <row r="47" spans="4:4">
+    <row r="47" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D47" s="1"/>
     </row>
-    <row r="48" spans="4:4">
+    <row r="48" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D48" s="1"/>
     </row>
-    <row r="49" spans="4:4">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D49" s="1"/>
     </row>
-    <row r="50" spans="4:4">
+    <row r="50" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D50" s="1"/>
     </row>
-    <row r="51" spans="4:4">
+    <row r="51" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D51" s="1"/>
     </row>
-    <row r="52" spans="4:4">
+    <row r="52" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D52" s="1"/>
     </row>
-    <row r="53" spans="4:4">
+    <row r="53" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D53" s="1"/>
     </row>
-    <row r="54" spans="4:4">
+    <row r="54" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D54" s="1"/>
     </row>
-    <row r="55" spans="4:4">
+    <row r="55" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D55" s="1"/>
     </row>
-    <row r="56" spans="4:4">
+    <row r="56" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D56" s="1"/>
     </row>
-    <row r="57" spans="4:4">
+    <row r="57" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D57" s="1"/>
     </row>
-    <row r="58" spans="4:4">
+    <row r="58" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D58" s="1"/>
     </row>
-    <row r="59" spans="4:4">
+    <row r="59" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D59" s="1"/>
     </row>
-    <row r="60" spans="4:4">
+    <row r="60" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D60" s="1"/>
     </row>
-    <row r="61" spans="4:4">
+    <row r="61" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D61" s="1"/>
     </row>
-    <row r="62" spans="4:4">
+    <row r="62" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D62" s="1"/>
     </row>
-    <row r="63" spans="4:4">
+    <row r="63" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D63" s="1"/>
     </row>
-    <row r="64" spans="4:4">
+    <row r="64" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D64" s="1"/>
     </row>
-    <row r="65" spans="4:4">
+    <row r="65" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D65" s="1"/>
     </row>
-    <row r="66" spans="4:4">
+    <row r="66" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D66" s="1"/>
     </row>
-    <row r="67" spans="4:4">
+    <row r="67" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D67" s="1"/>
     </row>
-    <row r="68" spans="4:4">
+    <row r="68" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D68" s="1"/>
     </row>
   </sheetData>
@@ -3387,22 +3456,22 @@
   <dimension ref="A1:J67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.33203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="47.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.83203125" style="3"/>
+    <col min="2" max="2" width="47.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.77734375" style="3"/>
     <col min="6" max="6" width="41.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.83203125" customWidth="1"/>
+    <col min="7" max="7" width="6.77734375" customWidth="1"/>
     <col min="8" max="8" width="20.6640625" customWidth="1"/>
-    <col min="9" max="9" width="21.83203125" customWidth="1"/>
+    <col min="9" max="9" width="21.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1">
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
@@ -3429,7 +3498,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>29</v>
       </c>
@@ -3457,7 +3526,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D3" s="7"/>
       <c r="H3" s="68" t="s">
         <v>45</v>
@@ -3468,7 +3537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15" thickBot="1">
+    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D4" s="8"/>
       <c r="H4" s="68" t="s">
         <v>46</v>
@@ -3479,7 +3548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15" thickBot="1">
+    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D5" s="1"/>
       <c r="H5" s="64" t="s">
         <v>16</v>
@@ -3490,19 +3559,19 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D6" s="8"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1">
+    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:10" ht="15" thickBot="1">
+    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D10" s="1"/>
       <c r="H10" s="41" t="s">
         <v>5</v>
@@ -3511,7 +3580,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D11" s="1"/>
       <c r="H11" s="42" t="s">
         <v>28</v>
@@ -3521,7 +3590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D12" s="1"/>
       <c r="H12" s="42" t="s">
         <v>6</v>
@@ -3531,7 +3600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15" thickBot="1">
+    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D13" s="1"/>
       <c r="H13" s="40" t="s">
         <v>29</v>
@@ -3541,370 +3610,370 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:10" s="3" customFormat="1">
+    <row r="16" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D16" s="1"/>
       <c r="G16"/>
       <c r="H16"/>
       <c r="I16"/>
       <c r="J16"/>
     </row>
-    <row r="17" spans="4:10" s="3" customFormat="1">
+    <row r="17" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D17" s="1"/>
       <c r="G17"/>
       <c r="H17"/>
       <c r="I17"/>
       <c r="J17"/>
     </row>
-    <row r="18" spans="4:10" s="3" customFormat="1">
+    <row r="18" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D18" s="1"/>
       <c r="G18"/>
       <c r="H18"/>
       <c r="I18"/>
       <c r="J18"/>
     </row>
-    <row r="19" spans="4:10" s="3" customFormat="1">
+    <row r="19" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D19" s="1"/>
       <c r="G19"/>
       <c r="H19"/>
       <c r="I19"/>
       <c r="J19"/>
     </row>
-    <row r="20" spans="4:10" s="3" customFormat="1">
+    <row r="20" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D20" s="1"/>
       <c r="G20"/>
       <c r="H20"/>
       <c r="I20"/>
       <c r="J20"/>
     </row>
-    <row r="21" spans="4:10" s="3" customFormat="1">
+    <row r="21" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D21" s="1"/>
       <c r="G21"/>
       <c r="H21"/>
       <c r="I21"/>
       <c r="J21"/>
     </row>
-    <row r="22" spans="4:10" s="3" customFormat="1">
+    <row r="22" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D22" s="1"/>
       <c r="G22"/>
       <c r="H22"/>
       <c r="I22"/>
       <c r="J22"/>
     </row>
-    <row r="23" spans="4:10" s="3" customFormat="1">
+    <row r="23" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D23" s="1"/>
       <c r="G23"/>
       <c r="H23"/>
       <c r="I23"/>
       <c r="J23"/>
     </row>
-    <row r="24" spans="4:10" s="3" customFormat="1">
+    <row r="24" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D24" s="1"/>
       <c r="G24"/>
       <c r="H24"/>
       <c r="I24"/>
       <c r="J24"/>
     </row>
-    <row r="25" spans="4:10" s="3" customFormat="1">
+    <row r="25" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D25" s="1"/>
       <c r="G25"/>
       <c r="H25"/>
       <c r="I25"/>
       <c r="J25"/>
     </row>
-    <row r="26" spans="4:10" s="3" customFormat="1">
+    <row r="26" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D26" s="1"/>
       <c r="G26"/>
       <c r="H26"/>
       <c r="I26"/>
       <c r="J26"/>
     </row>
-    <row r="27" spans="4:10" s="3" customFormat="1">
+    <row r="27" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D27" s="1"/>
       <c r="G27"/>
       <c r="H27"/>
       <c r="I27"/>
       <c r="J27"/>
     </row>
-    <row r="28" spans="4:10" s="3" customFormat="1">
+    <row r="28" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D28" s="1"/>
       <c r="G28"/>
       <c r="H28"/>
       <c r="I28"/>
       <c r="J28"/>
     </row>
-    <row r="29" spans="4:10" s="3" customFormat="1">
+    <row r="29" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D29" s="1"/>
       <c r="G29"/>
       <c r="H29"/>
       <c r="I29"/>
       <c r="J29"/>
     </row>
-    <row r="30" spans="4:10" s="3" customFormat="1">
+    <row r="30" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D30" s="1"/>
       <c r="G30"/>
       <c r="H30"/>
       <c r="I30"/>
       <c r="J30"/>
     </row>
-    <row r="31" spans="4:10" s="3" customFormat="1">
+    <row r="31" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D31" s="1"/>
       <c r="G31"/>
       <c r="H31"/>
       <c r="I31"/>
       <c r="J31"/>
     </row>
-    <row r="32" spans="4:10" s="3" customFormat="1">
+    <row r="32" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D32" s="1"/>
       <c r="G32"/>
       <c r="H32"/>
       <c r="I32"/>
       <c r="J32"/>
     </row>
-    <row r="33" spans="4:10" s="3" customFormat="1">
+    <row r="33" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D33" s="1"/>
       <c r="G33"/>
       <c r="H33"/>
       <c r="I33"/>
       <c r="J33"/>
     </row>
-    <row r="34" spans="4:10" s="3" customFormat="1">
+    <row r="34" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D34" s="1"/>
       <c r="G34"/>
       <c r="H34"/>
       <c r="I34"/>
       <c r="J34"/>
     </row>
-    <row r="35" spans="4:10" s="3" customFormat="1">
+    <row r="35" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D35" s="1"/>
       <c r="G35"/>
       <c r="H35"/>
       <c r="I35"/>
       <c r="J35"/>
     </row>
-    <row r="36" spans="4:10" s="3" customFormat="1">
+    <row r="36" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D36" s="1"/>
       <c r="G36"/>
       <c r="H36"/>
       <c r="I36"/>
       <c r="J36"/>
     </row>
-    <row r="37" spans="4:10" s="3" customFormat="1">
+    <row r="37" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D37" s="1"/>
       <c r="G37"/>
       <c r="H37"/>
       <c r="I37"/>
       <c r="J37"/>
     </row>
-    <row r="38" spans="4:10" s="3" customFormat="1">
+    <row r="38" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D38" s="1"/>
       <c r="G38"/>
       <c r="H38"/>
       <c r="I38"/>
       <c r="J38"/>
     </row>
-    <row r="39" spans="4:10" s="3" customFormat="1">
+    <row r="39" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D39" s="1"/>
       <c r="G39"/>
       <c r="H39"/>
       <c r="I39"/>
       <c r="J39"/>
     </row>
-    <row r="40" spans="4:10" s="3" customFormat="1">
+    <row r="40" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D40" s="1"/>
       <c r="G40"/>
       <c r="H40"/>
       <c r="I40"/>
       <c r="J40"/>
     </row>
-    <row r="41" spans="4:10" s="3" customFormat="1">
+    <row r="41" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D41" s="1"/>
       <c r="G41"/>
       <c r="H41"/>
       <c r="I41"/>
       <c r="J41"/>
     </row>
-    <row r="42" spans="4:10" s="3" customFormat="1">
+    <row r="42" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D42" s="1"/>
       <c r="G42"/>
       <c r="H42"/>
       <c r="I42"/>
       <c r="J42"/>
     </row>
-    <row r="43" spans="4:10" s="3" customFormat="1">
+    <row r="43" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D43" s="1"/>
       <c r="G43"/>
       <c r="H43"/>
       <c r="I43"/>
       <c r="J43"/>
     </row>
-    <row r="44" spans="4:10" s="3" customFormat="1">
+    <row r="44" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D44" s="1"/>
       <c r="G44"/>
       <c r="H44"/>
       <c r="I44"/>
       <c r="J44"/>
     </row>
-    <row r="45" spans="4:10" s="3" customFormat="1">
+    <row r="45" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D45" s="1"/>
       <c r="G45"/>
       <c r="H45"/>
       <c r="I45"/>
       <c r="J45"/>
     </row>
-    <row r="46" spans="4:10" s="3" customFormat="1">
+    <row r="46" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D46" s="1"/>
       <c r="G46"/>
       <c r="H46"/>
       <c r="I46"/>
       <c r="J46"/>
     </row>
-    <row r="47" spans="4:10" s="3" customFormat="1">
+    <row r="47" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D47" s="1"/>
       <c r="G47"/>
       <c r="H47"/>
       <c r="I47"/>
       <c r="J47"/>
     </row>
-    <row r="48" spans="4:10" s="3" customFormat="1">
+    <row r="48" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D48" s="1"/>
       <c r="G48"/>
       <c r="H48"/>
       <c r="I48"/>
       <c r="J48"/>
     </row>
-    <row r="49" spans="4:10" s="3" customFormat="1">
+    <row r="49" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D49" s="1"/>
       <c r="G49"/>
       <c r="H49"/>
       <c r="I49"/>
       <c r="J49"/>
     </row>
-    <row r="50" spans="4:10" s="3" customFormat="1">
+    <row r="50" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D50" s="1"/>
       <c r="G50"/>
       <c r="H50"/>
       <c r="I50"/>
       <c r="J50"/>
     </row>
-    <row r="51" spans="4:10" s="3" customFormat="1">
+    <row r="51" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D51" s="1"/>
       <c r="G51"/>
       <c r="H51"/>
       <c r="I51"/>
       <c r="J51"/>
     </row>
-    <row r="52" spans="4:10" s="3" customFormat="1">
+    <row r="52" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D52" s="1"/>
       <c r="G52"/>
       <c r="H52"/>
       <c r="I52"/>
       <c r="J52"/>
     </row>
-    <row r="53" spans="4:10" s="3" customFormat="1">
+    <row r="53" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D53" s="1"/>
       <c r="G53"/>
       <c r="H53"/>
       <c r="I53"/>
       <c r="J53"/>
     </row>
-    <row r="54" spans="4:10" s="3" customFormat="1">
+    <row r="54" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D54" s="1"/>
       <c r="G54"/>
       <c r="H54"/>
       <c r="I54"/>
       <c r="J54"/>
     </row>
-    <row r="55" spans="4:10" s="3" customFormat="1">
+    <row r="55" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D55" s="1"/>
       <c r="G55"/>
       <c r="H55"/>
       <c r="I55"/>
       <c r="J55"/>
     </row>
-    <row r="56" spans="4:10" s="3" customFormat="1">
+    <row r="56" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D56" s="1"/>
       <c r="G56"/>
       <c r="H56"/>
       <c r="I56"/>
       <c r="J56"/>
     </row>
-    <row r="57" spans="4:10" s="3" customFormat="1">
+    <row r="57" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D57" s="1"/>
       <c r="G57"/>
       <c r="H57"/>
       <c r="I57"/>
       <c r="J57"/>
     </row>
-    <row r="58" spans="4:10" s="3" customFormat="1">
+    <row r="58" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D58" s="1"/>
       <c r="G58"/>
       <c r="H58"/>
       <c r="I58"/>
       <c r="J58"/>
     </row>
-    <row r="59" spans="4:10" s="3" customFormat="1">
+    <row r="59" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D59" s="1"/>
       <c r="G59"/>
       <c r="H59"/>
       <c r="I59"/>
       <c r="J59"/>
     </row>
-    <row r="60" spans="4:10" s="3" customFormat="1">
+    <row r="60" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D60" s="1"/>
       <c r="G60"/>
       <c r="H60"/>
       <c r="I60"/>
       <c r="J60"/>
     </row>
-    <row r="61" spans="4:10" s="3" customFormat="1">
+    <row r="61" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D61" s="1"/>
       <c r="G61"/>
       <c r="H61"/>
       <c r="I61"/>
       <c r="J61"/>
     </row>
-    <row r="62" spans="4:10" s="3" customFormat="1">
+    <row r="62" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D62" s="1"/>
       <c r="G62"/>
       <c r="H62"/>
       <c r="I62"/>
       <c r="J62"/>
     </row>
-    <row r="63" spans="4:10" s="3" customFormat="1">
+    <row r="63" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D63" s="1"/>
       <c r="G63"/>
       <c r="H63"/>
       <c r="I63"/>
       <c r="J63"/>
     </row>
-    <row r="64" spans="4:10" s="3" customFormat="1">
+    <row r="64" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D64" s="1"/>
       <c r="G64"/>
       <c r="H64"/>
       <c r="I64"/>
       <c r="J64"/>
     </row>
-    <row r="65" spans="4:10" s="3" customFormat="1">
+    <row r="65" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D65" s="1"/>
       <c r="G65"/>
       <c r="H65"/>
       <c r="I65"/>
       <c r="J65"/>
     </row>
-    <row r="66" spans="4:10" s="3" customFormat="1">
+    <row r="66" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D66" s="1"/>
       <c r="G66"/>
       <c r="H66"/>
       <c r="I66"/>
       <c r="J66"/>
     </row>
-    <row r="67" spans="4:10" s="3" customFormat="1">
+    <row r="67" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D67" s="1"/>
       <c r="G67"/>
       <c r="H67"/>
@@ -3944,19 +4013,19 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" style="3" customWidth="1"/>
     <col min="3" max="3" width="86.6640625" style="3" customWidth="1"/>
-    <col min="4" max="5" width="10.83203125" style="3"/>
-    <col min="6" max="6" width="45.83203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="7.1640625" customWidth="1"/>
-    <col min="8" max="8" width="15.1640625" customWidth="1"/>
-    <col min="9" max="9" width="16.1640625" customWidth="1"/>
+    <col min="4" max="5" width="10.77734375" style="3"/>
+    <col min="6" max="6" width="45.77734375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="7.109375" customWidth="1"/>
+    <col min="8" max="8" width="15.109375" customWidth="1"/>
+    <col min="9" max="9" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1">
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
@@ -3983,7 +4052,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D2" s="1"/>
       <c r="H2" s="70" t="s">
         <v>47</v>
@@ -3994,7 +4063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D3" s="1"/>
       <c r="H3" s="68" t="s">
         <v>48</v>
@@ -4005,7 +4074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D4" s="1"/>
       <c r="H4" s="68" t="s">
         <v>49</v>
@@ -4016,7 +4085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D5" s="1"/>
       <c r="H5" s="68" t="s">
         <v>50</v>
@@ -4027,7 +4096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D6" s="1"/>
       <c r="H6" s="72" t="s">
         <v>51</v>
@@ -4038,7 +4107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15" thickBot="1">
+    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D7" s="1"/>
       <c r="H7" s="74" t="s">
         <v>52</v>
@@ -4049,7 +4118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1">
+    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D8" s="1"/>
       <c r="H8" s="64" t="s">
         <v>16</v>
@@ -4060,16 +4129,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:10" ht="15" thickBot="1">
+    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:10" ht="15" thickBot="1">
+    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H12" s="6" t="s">
         <v>5</v>
       </c>
@@ -4077,7 +4146,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H13" s="35" t="s">
         <v>28</v>
       </c>
@@ -4086,7 +4155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H14" s="35" t="s">
         <v>6</v>
       </c>
@@ -4095,7 +4164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1">
+    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H15" s="34" t="s">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
Added Dictionary Attribute & Updated Zeitaufzeichnung
</commit_message>
<xml_diff>
--- a/Dokumentation/Aquila_Zeitaufzeichnung.xlsx
+++ b/Dokumentation/Aquila_Zeitaufzeichnung.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="3204" yWindow="0" windowWidth="20736" windowHeight="11760" activeTab="3"/>
+    <workbookView xWindow="3204" yWindow="0" windowWidth="20736" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Gesamtstatus" sheetId="4" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="133">
   <si>
     <t>Arbeitspaket</t>
   </si>
@@ -411,6 +411,18 @@
   </si>
   <si>
     <t>Aktualisierte Seitenstruktur &amp; Jquery-Suche</t>
+  </si>
+  <si>
+    <t>Worker-Thread Prototyp</t>
+  </si>
+  <si>
+    <t>WCF-Prototyp implementiert</t>
+  </si>
+  <si>
+    <t>WCF-Prototyp</t>
+  </si>
+  <si>
+    <t>Worker-Thread Prototyp implementiert</t>
   </si>
 </sst>
 </file>
@@ -976,12 +988,12 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:shape val="box"/>
-        <c:axId val="39081856"/>
-        <c:axId val="39083392"/>
+        <c:axId val="38094720"/>
+        <c:axId val="38096256"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="39081856"/>
+        <c:axId val="38094720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -990,7 +1002,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39083392"/>
+        <c:crossAx val="38096256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -998,7 +1010,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39083392"/>
+        <c:axId val="38096256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1014,7 +1026,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="39081856"/>
+        <c:crossAx val="38094720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1139,7 +1151,7 @@
                   <c:v>14.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23.5</c:v>
+                  <c:v>29.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1155,12 +1167,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="39116800"/>
-        <c:axId val="39118336"/>
+        <c:axId val="38133760"/>
+        <c:axId val="38135296"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="39116800"/>
+        <c:axId val="38133760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1169,7 +1181,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39118336"/>
+        <c:crossAx val="38135296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1177,7 +1189,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39118336"/>
+        <c:axId val="38135296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1188,7 +1200,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39116800"/>
+        <c:crossAx val="38133760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1559,8 +1571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1596,7 +1608,7 @@
       </c>
       <c r="B3" s="10">
         <f>SUM(B6,B12,B17)</f>
-        <v>30.5</v>
+        <v>36.5</v>
       </c>
       <c r="C3" s="28">
         <v>1</v>
@@ -1695,7 +1707,7 @@
       </c>
       <c r="B12" s="19">
         <f>Software!J6</f>
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C12" s="30">
         <v>1</v>
@@ -1710,7 +1722,7 @@
       </c>
       <c r="B13" s="24">
         <f>Software!J2</f>
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C13" s="32"/>
       <c r="D13" s="33"/>
@@ -1813,7 +1825,7 @@
       </c>
       <c r="B22" s="19">
         <f>Schnittstellen!J5</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C22" s="30">
         <v>1</v>
@@ -1850,7 +1862,7 @@
       </c>
       <c r="B25" s="24">
         <f>Schnittstellen!J4</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C25" s="32"/>
       <c r="D25" s="33"/>
@@ -1971,7 +1983,7 @@
       <c r="C37" s="51"/>
       <c r="D37" s="40">
         <f>SUM(Projektmanagement!I15,Software!I14,Website!I14,Schnittstellen!J13,'Testing &amp; Abschluss'!I15)</f>
-        <v>23.5</v>
+        <v>29.5</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2288,7 +2300,7 @@
   <dimension ref="A1:J68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2354,7 +2366,7 @@
       <c r="I2" s="71"/>
       <c r="J2" s="4">
         <f>SUMIF(B:B,H2,E:E)</f>
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -2466,7 +2478,7 @@
       <c r="I6" s="69"/>
       <c r="J6" s="10">
         <f>SUM(J2:J5)</f>
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -2510,7 +2522,24 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="D9" s="7"/>
+      <c r="A9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D9" s="7">
+        <v>41318</v>
+      </c>
+      <c r="E9" s="3">
+        <v>6</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D10" s="1"/>
@@ -2551,7 +2580,7 @@
       </c>
       <c r="I14" s="34">
         <f>SUMIF(A:A,H14,E:E)</f>
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -2746,7 +2775,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
@@ -3471,7 +3500,7 @@
   <dimension ref="A1:J67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3542,7 +3571,24 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="D3" s="7"/>
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D3" s="7">
+        <v>41318</v>
+      </c>
+      <c r="E3" s="3">
+        <v>6</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>131</v>
+      </c>
       <c r="H3" s="68" t="s">
         <v>45</v>
       </c>
@@ -3560,7 +3606,7 @@
       <c r="I4" s="68"/>
       <c r="J4" s="42">
         <f>SUMIF(B:B,H4,E:E)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3571,7 +3617,7 @@
       <c r="I5" s="69"/>
       <c r="J5" s="10">
         <f>SUM(J2:J4)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -3612,7 +3658,7 @@
       </c>
       <c r="I12" s="42">
         <f>SUMIF(A:A,H12,E:E)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated Server and ZeiAquila_Zeitaufzeichnung
</commit_message>
<xml_diff>
--- a/Dokumentation/Aquila_Zeitaufzeichnung.xlsx
+++ b/Dokumentation/Aquila_Zeitaufzeichnung.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="10230" yWindow="-15" windowWidth="10275" windowHeight="8325" activeTab="1"/>
+    <workbookView xWindow="10236" yWindow="-12" windowWidth="10272" windowHeight="8328" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Gesamtstatus" sheetId="4" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="155">
   <si>
     <t>Arbeitspaket</t>
   </si>
@@ -483,6 +483,12 @@
   </si>
   <si>
     <t>ein weiterer Fehler gefunden (DataContract)</t>
+  </si>
+  <si>
+    <t>neues WCF-Konzept</t>
+  </si>
+  <si>
+    <t>Erste vollstänfg funktionierende WCF-Verbindung</t>
   </si>
 </sst>
 </file>
@@ -965,7 +971,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1053,12 +1058,12 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:shape val="box"/>
-        <c:axId val="85958016"/>
-        <c:axId val="85959808"/>
+        <c:axId val="6116864"/>
+        <c:axId val="6118400"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="85958016"/>
+        <c:axId val="6116864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1067,7 +1072,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85959808"/>
+        <c:crossAx val="6118400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1075,7 +1080,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="85959808"/>
+        <c:axId val="6118400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1091,7 +1096,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="85958016"/>
+        <c:crossAx val="6116864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1126,7 +1131,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1205,7 +1209,7 @@
                   <c:v>104.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>48.5</c:v>
@@ -1224,12 +1228,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="88278144"/>
-        <c:axId val="88279680"/>
+        <c:axId val="6151168"/>
+        <c:axId val="6152960"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="88278144"/>
+        <c:axId val="6151168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1238,7 +1242,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88279680"/>
+        <c:crossAx val="6152960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1246,7 +1250,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88279680"/>
+        <c:axId val="6152960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1257,7 +1261,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88278144"/>
+        <c:crossAx val="6151168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1632,13 +1636,13 @@
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="45" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="55"/>
       <c r="B1" s="57" t="s">
         <v>24</v>
@@ -1649,7 +1653,7 @@
       <c r="D1" s="52"/>
       <c r="O1" s="11"/>
     </row>
-    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="56"/>
       <c r="B2" s="58"/>
       <c r="C2" s="15" t="s">
@@ -1674,7 +1678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="52"/>
       <c r="B4" s="57"/>
       <c r="C4" s="59" t="s">
@@ -1682,13 +1686,13 @@
       </c>
       <c r="D4" s="60"/>
     </row>
-    <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="56"/>
       <c r="B5" s="58"/>
       <c r="C5" s="61"/>
       <c r="D5" s="62"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>12</v>
       </c>
@@ -1703,7 +1707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>18</v>
       </c>
@@ -1714,7 +1718,7 @@
       <c r="C7" s="31"/>
       <c r="D7" s="32"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>17</v>
       </c>
@@ -1725,7 +1729,7 @@
       <c r="C8" s="31"/>
       <c r="D8" s="32"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>19</v>
       </c>
@@ -1736,7 +1740,7 @@
       <c r="C9" s="31"/>
       <c r="D9" s="32"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>20</v>
       </c>
@@ -1758,7 +1762,7 @@
       <c r="C11" s="27"/>
       <c r="D11" s="28"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="44" t="s">
         <v>65</v>
       </c>
@@ -1773,7 +1777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="42" t="s">
         <v>57</v>
       </c>
@@ -1784,7 +1788,7 @@
       <c r="C13" s="31"/>
       <c r="D13" s="32"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="42" t="s">
         <v>58</v>
       </c>
@@ -1795,7 +1799,7 @@
       <c r="C14" s="31"/>
       <c r="D14" s="32"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="42" t="s">
         <v>59</v>
       </c>
@@ -1817,7 +1821,7 @@
       <c r="C16" s="31"/>
       <c r="D16" s="32"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="44" t="s">
         <v>66</v>
       </c>
@@ -1832,7 +1836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="42" t="s">
         <v>61</v>
       </c>
@@ -1843,7 +1847,7 @@
       <c r="C18" s="31"/>
       <c r="D18" s="32"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="42" t="s">
         <v>62</v>
       </c>
@@ -1854,7 +1858,7 @@
       <c r="C19" s="31"/>
       <c r="D19" s="32"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="42" t="s">
         <v>63</v>
       </c>
@@ -1876,13 +1880,13 @@
       <c r="C21" s="27"/>
       <c r="D21" s="28"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="44" t="s">
         <v>67</v>
       </c>
       <c r="B22" s="19">
         <f>Schnittstellen!J5</f>
-        <v>44.5</v>
+        <v>48.5</v>
       </c>
       <c r="C22" s="29">
         <v>1</v>
@@ -1891,7 +1895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="42" t="s">
         <v>68</v>
       </c>
@@ -1902,7 +1906,7 @@
       <c r="C23" s="31"/>
       <c r="D23" s="32"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="42" t="s">
         <v>69</v>
       </c>
@@ -1919,12 +1923,12 @@
       </c>
       <c r="B25" s="24">
         <f>Schnittstellen!J4</f>
-        <v>31.5</v>
+        <v>35.5</v>
       </c>
       <c r="C25" s="31"/>
       <c r="D25" s="32"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="44" t="s">
         <v>13</v>
       </c>
@@ -1939,7 +1943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="42" t="s">
         <v>71</v>
       </c>
@@ -1950,7 +1954,7 @@
       <c r="C27" s="31"/>
       <c r="D27" s="32"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="42" t="s">
         <v>72</v>
       </c>
@@ -1961,7 +1965,7 @@
       <c r="C28" s="31"/>
       <c r="D28" s="32"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="42" t="s">
         <v>73</v>
       </c>
@@ -1972,7 +1976,7 @@
       <c r="C29" s="31"/>
       <c r="D29" s="32"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="42" t="s">
         <v>74</v>
       </c>
@@ -1983,7 +1987,7 @@
       <c r="C30" s="31"/>
       <c r="D30" s="32"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="42" t="s">
         <v>75</v>
       </c>
@@ -1994,7 +1998,7 @@
       <c r="C31" s="31"/>
       <c r="D31" s="32"/>
     </row>
-    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="43" t="s">
         <v>76</v>
       </c>
@@ -2023,14 +2027,14 @@
         <v>104.5</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B36" s="47" t="s">
         <v>15</v>
       </c>
       <c r="C36" s="48"/>
       <c r="D36" s="41">
         <f>SUM(Projektmanagement!I14,Software!I13,Website!I13,Schnittstellen!I12,'Testing &amp; Abschluss'!I14)</f>
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2070,19 +2074,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="71.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" style="3"/>
-    <col min="5" max="5" width="10.85546875" style="26"/>
-    <col min="6" max="6" width="24.42578125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="71.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" style="3"/>
+    <col min="5" max="5" width="10.88671875" style="26"/>
+    <col min="6" max="6" width="24.44140625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2112,7 +2116,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2140,7 +2144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -2168,7 +2172,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -2196,7 +2200,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -2280,7 +2284,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -2300,7 +2304,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
@@ -2320,7 +2324,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
@@ -2352,7 +2356,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D13" s="1"/>
       <c r="H13" s="34" t="s">
         <v>28</v>
@@ -2362,7 +2366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D14" s="1"/>
       <c r="H14" s="34" t="s">
         <v>6</v>
@@ -2382,15 +2386,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D16" s="1"/>
       <c r="H16" s="38"/>
       <c r="I16" s="38"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:4" ht="15" x14ac:dyDescent="0.25">
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:4" ht="15" x14ac:dyDescent="0.25">
       <c r="D18" s="1"/>
     </row>
   </sheetData>
@@ -2424,19 +2428,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J68"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="45.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.85546875" style="3"/>
-    <col min="6" max="6" width="41.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="31.44140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="45.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.88671875" style="3"/>
+    <col min="6" max="6" width="41.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" customWidth="1"/>
+    <col min="9" max="9" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2466,7 +2470,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>29</v>
       </c>
@@ -2494,7 +2498,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>29</v>
       </c>
@@ -2522,7 +2526,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -2606,7 +2610,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>29</v>
       </c>
@@ -2626,7 +2630,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>29</v>
       </c>
@@ -2646,7 +2650,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>29</v>
       </c>
@@ -2678,7 +2682,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D12" s="1"/>
       <c r="H12" s="4" t="s">
         <v>28</v>
@@ -2688,7 +2692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D13" s="1"/>
       <c r="H13" s="4" t="s">
         <v>6</v>
@@ -2708,166 +2712,166 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:4" ht="15" x14ac:dyDescent="0.25">
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:4" ht="15" x14ac:dyDescent="0.25">
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:4" ht="15" x14ac:dyDescent="0.25">
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:4" ht="15" x14ac:dyDescent="0.25">
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:4" ht="15" x14ac:dyDescent="0.25">
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:4" ht="15" x14ac:dyDescent="0.25">
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:4" ht="15" x14ac:dyDescent="0.25">
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:4" ht="15" x14ac:dyDescent="0.25">
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:4" ht="15" x14ac:dyDescent="0.25">
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:4" ht="15" x14ac:dyDescent="0.25">
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:4" ht="15" x14ac:dyDescent="0.25">
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:4" ht="15" x14ac:dyDescent="0.25">
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:4" ht="15" x14ac:dyDescent="0.25">
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:4" ht="15" x14ac:dyDescent="0.25">
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:4" ht="15" x14ac:dyDescent="0.25">
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D32" s="1"/>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D33" s="1"/>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D34" s="1"/>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D35" s="1"/>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D36" s="1"/>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D37" s="1"/>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D38" s="1"/>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D40" s="1"/>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D41" s="1"/>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D42" s="1"/>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D43" s="1"/>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D44" s="1"/>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D45" s="1"/>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D46" s="1"/>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D47" s="1"/>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D48" s="1"/>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D49" s="1"/>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D50" s="1"/>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D51" s="1"/>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D52" s="1"/>
     </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D53" s="1"/>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D54" s="1"/>
     </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D55" s="1"/>
     </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D56" s="1"/>
     </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D57" s="1"/>
     </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D58" s="1"/>
     </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D59" s="1"/>
     </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D60" s="1"/>
     </row>
-    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D61" s="1"/>
     </row>
-    <row r="62" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D62" s="1"/>
     </row>
-    <row r="63" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D63" s="1"/>
     </row>
-    <row r="64" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D64" s="1"/>
     </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D65" s="1"/>
     </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D66" s="1"/>
     </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D67" s="1"/>
     </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D68" s="1"/>
     </row>
   </sheetData>
@@ -2904,16 +2908,16 @@
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" style="3" customWidth="1"/>
     <col min="2" max="2" width="30" style="3" customWidth="1"/>
-    <col min="3" max="3" width="45.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" style="3"/>
-    <col min="5" max="5" width="10.85546875" style="46"/>
-    <col min="6" max="6" width="41.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="45.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" style="3"/>
+    <col min="5" max="5" width="10.88671875" style="46"/>
+    <col min="6" max="6" width="41.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" customWidth="1"/>
+    <col min="9" max="9" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2943,7 +2947,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>28</v>
       </c>
@@ -2971,7 +2975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>28</v>
       </c>
@@ -2999,7 +3003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>28</v>
       </c>
@@ -3027,7 +3031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>28</v>
       </c>
@@ -3055,7 +3059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>28</v>
       </c>
@@ -3080,7 +3084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>29</v>
       </c>
@@ -3097,7 +3101,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>28</v>
       </c>
@@ -3114,7 +3118,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>28</v>
       </c>
@@ -3154,7 +3158,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>29</v>
       </c>
@@ -3180,7 +3184,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>28</v>
       </c>
@@ -3207,7 +3211,7 @@
         <v>91.5</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>28</v>
       </c>
@@ -3261,7 +3265,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>28</v>
       </c>
@@ -3281,7 +3285,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>28</v>
       </c>
@@ -3301,7 +3305,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>28</v>
       </c>
@@ -3321,7 +3325,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>28</v>
       </c>
@@ -3341,7 +3345,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>29</v>
       </c>
@@ -3361,7 +3365,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>28</v>
       </c>
@@ -3381,7 +3385,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>28</v>
       </c>
@@ -3401,7 +3405,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>28</v>
       </c>
@@ -3421,7 +3425,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>28</v>
       </c>
@@ -3441,7 +3445,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>28</v>
       </c>
@@ -3461,7 +3465,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>28</v>
       </c>
@@ -3481,7 +3485,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>28</v>
       </c>
@@ -3501,7 +3505,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>28</v>
       </c>
@@ -3521,7 +3525,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>28</v>
       </c>
@@ -3541,121 +3545,121 @@
         <v>147</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="D32" s="1"/>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:4" ht="15" x14ac:dyDescent="0.25">
       <c r="D33" s="1"/>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:4" ht="15" x14ac:dyDescent="0.25">
       <c r="D34" s="1"/>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:4" ht="15" x14ac:dyDescent="0.25">
       <c r="D35" s="1"/>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:4" ht="15" x14ac:dyDescent="0.25">
       <c r="D36" s="1"/>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:4" ht="15" x14ac:dyDescent="0.25">
       <c r="D37" s="1"/>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:4" ht="15" x14ac:dyDescent="0.25">
       <c r="D38" s="1"/>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:4" ht="15" x14ac:dyDescent="0.25">
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:4" ht="15" x14ac:dyDescent="0.25">
       <c r="D40" s="1"/>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D41" s="1"/>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D42" s="1"/>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D43" s="1"/>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D44" s="1"/>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D45" s="1"/>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D46" s="1"/>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D47" s="1"/>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D48" s="1"/>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D49" s="1"/>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D50" s="1"/>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D51" s="1"/>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D52" s="1"/>
     </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D53" s="1"/>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D54" s="1"/>
     </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D55" s="1"/>
     </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D56" s="1"/>
     </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D57" s="1"/>
     </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D58" s="1"/>
     </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D59" s="1"/>
     </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D60" s="1"/>
     </row>
-    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D61" s="1"/>
     </row>
-    <row r="62" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D62" s="1"/>
     </row>
-    <row r="63" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D63" s="1"/>
     </row>
-    <row r="64" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D64" s="1"/>
     </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D65" s="1"/>
     </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D66" s="1"/>
     </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D67" s="1"/>
     </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D68" s="1"/>
     </row>
   </sheetData>
@@ -3688,20 +3692,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="47.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.85546875" style="3"/>
-    <col min="6" max="6" width="41.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" customWidth="1"/>
-    <col min="9" max="9" width="21.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="47.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.88671875" style="3"/>
+    <col min="6" max="6" width="41.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.6640625" customWidth="1"/>
+    <col min="8" max="8" width="20.6640625" customWidth="1"/>
+    <col min="9" max="9" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3731,7 +3735,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>29</v>
       </c>
@@ -3759,7 +3763,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>28</v>
       </c>
@@ -3812,7 +3816,7 @@
       <c r="I4" s="67"/>
       <c r="J4" s="41">
         <f>SUMIF(B:B,H4,E:E)</f>
-        <v>31.5</v>
+        <v>35.5</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3840,10 +3844,10 @@
       <c r="I5" s="68"/>
       <c r="J5" s="10">
         <f>SUM(J2:J4)</f>
-        <v>44.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>48.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>29</v>
       </c>
@@ -3863,7 +3867,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -3883,7 +3887,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>28</v>
       </c>
@@ -3949,7 +3953,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>29</v>
       </c>
@@ -3976,7 +3980,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>29</v>
       </c>
@@ -4000,11 +4004,28 @@
       </c>
       <c r="I12" s="41">
         <f>SUMIF(A:A,H12,E:E)</f>
-        <v>12.5</v>
+        <v>16.5</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D13" s="1"/>
+      <c r="A13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D13" s="1">
+        <v>41340</v>
+      </c>
+      <c r="E13" s="3">
+        <v>4</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>154</v>
+      </c>
       <c r="H13" s="39" t="s">
         <v>29</v>
       </c>
@@ -4013,370 +4034,370 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="D16" s="1"/>
       <c r="G16"/>
       <c r="H16"/>
       <c r="I16"/>
       <c r="J16"/>
     </row>
-    <row r="17" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="D17" s="1"/>
       <c r="G17"/>
       <c r="H17"/>
       <c r="I17"/>
       <c r="J17"/>
     </row>
-    <row r="18" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="D18" s="1"/>
       <c r="G18"/>
       <c r="H18"/>
       <c r="I18"/>
       <c r="J18"/>
     </row>
-    <row r="19" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="D19" s="1"/>
       <c r="G19"/>
       <c r="H19"/>
       <c r="I19"/>
       <c r="J19"/>
     </row>
-    <row r="20" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="D20" s="1"/>
       <c r="G20"/>
       <c r="H20"/>
       <c r="I20"/>
       <c r="J20"/>
     </row>
-    <row r="21" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="D21" s="1"/>
       <c r="G21"/>
       <c r="H21"/>
       <c r="I21"/>
       <c r="J21"/>
     </row>
-    <row r="22" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="D22" s="1"/>
       <c r="G22"/>
       <c r="H22"/>
       <c r="I22"/>
       <c r="J22"/>
     </row>
-    <row r="23" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="D23" s="1"/>
       <c r="G23"/>
       <c r="H23"/>
       <c r="I23"/>
       <c r="J23"/>
     </row>
-    <row r="24" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="D24" s="1"/>
       <c r="G24"/>
       <c r="H24"/>
       <c r="I24"/>
       <c r="J24"/>
     </row>
-    <row r="25" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="D25" s="1"/>
       <c r="G25"/>
       <c r="H25"/>
       <c r="I25"/>
       <c r="J25"/>
     </row>
-    <row r="26" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="D26" s="1"/>
       <c r="G26"/>
       <c r="H26"/>
       <c r="I26"/>
       <c r="J26"/>
     </row>
-    <row r="27" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="D27" s="1"/>
       <c r="G27"/>
       <c r="H27"/>
       <c r="I27"/>
       <c r="J27"/>
     </row>
-    <row r="28" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="D28" s="1"/>
       <c r="G28"/>
       <c r="H28"/>
       <c r="I28"/>
       <c r="J28"/>
     </row>
-    <row r="29" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="D29" s="1"/>
       <c r="G29"/>
       <c r="H29"/>
       <c r="I29"/>
       <c r="J29"/>
     </row>
-    <row r="30" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="D30" s="1"/>
       <c r="G30"/>
       <c r="H30"/>
       <c r="I30"/>
       <c r="J30"/>
     </row>
-    <row r="31" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="D31" s="1"/>
       <c r="G31"/>
       <c r="H31"/>
       <c r="I31"/>
       <c r="J31"/>
     </row>
-    <row r="32" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D32" s="1"/>
       <c r="G32"/>
       <c r="H32"/>
       <c r="I32"/>
       <c r="J32"/>
     </row>
-    <row r="33" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D33" s="1"/>
       <c r="G33"/>
       <c r="H33"/>
       <c r="I33"/>
       <c r="J33"/>
     </row>
-    <row r="34" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D34" s="1"/>
       <c r="G34"/>
       <c r="H34"/>
       <c r="I34"/>
       <c r="J34"/>
     </row>
-    <row r="35" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D35" s="1"/>
       <c r="G35"/>
       <c r="H35"/>
       <c r="I35"/>
       <c r="J35"/>
     </row>
-    <row r="36" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D36" s="1"/>
       <c r="G36"/>
       <c r="H36"/>
       <c r="I36"/>
       <c r="J36"/>
     </row>
-    <row r="37" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D37" s="1"/>
       <c r="G37"/>
       <c r="H37"/>
       <c r="I37"/>
       <c r="J37"/>
     </row>
-    <row r="38" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D38" s="1"/>
       <c r="G38"/>
       <c r="H38"/>
       <c r="I38"/>
       <c r="J38"/>
     </row>
-    <row r="39" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D39" s="1"/>
       <c r="G39"/>
       <c r="H39"/>
       <c r="I39"/>
       <c r="J39"/>
     </row>
-    <row r="40" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D40" s="1"/>
       <c r="G40"/>
       <c r="H40"/>
       <c r="I40"/>
       <c r="J40"/>
     </row>
-    <row r="41" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D41" s="1"/>
       <c r="G41"/>
       <c r="H41"/>
       <c r="I41"/>
       <c r="J41"/>
     </row>
-    <row r="42" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D42" s="1"/>
       <c r="G42"/>
       <c r="H42"/>
       <c r="I42"/>
       <c r="J42"/>
     </row>
-    <row r="43" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D43" s="1"/>
       <c r="G43"/>
       <c r="H43"/>
       <c r="I43"/>
       <c r="J43"/>
     </row>
-    <row r="44" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D44" s="1"/>
       <c r="G44"/>
       <c r="H44"/>
       <c r="I44"/>
       <c r="J44"/>
     </row>
-    <row r="45" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D45" s="1"/>
       <c r="G45"/>
       <c r="H45"/>
       <c r="I45"/>
       <c r="J45"/>
     </row>
-    <row r="46" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D46" s="1"/>
       <c r="G46"/>
       <c r="H46"/>
       <c r="I46"/>
       <c r="J46"/>
     </row>
-    <row r="47" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D47" s="1"/>
       <c r="G47"/>
       <c r="H47"/>
       <c r="I47"/>
       <c r="J47"/>
     </row>
-    <row r="48" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D48" s="1"/>
       <c r="G48"/>
       <c r="H48"/>
       <c r="I48"/>
       <c r="J48"/>
     </row>
-    <row r="49" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D49" s="1"/>
       <c r="G49"/>
       <c r="H49"/>
       <c r="I49"/>
       <c r="J49"/>
     </row>
-    <row r="50" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D50" s="1"/>
       <c r="G50"/>
       <c r="H50"/>
       <c r="I50"/>
       <c r="J50"/>
     </row>
-    <row r="51" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D51" s="1"/>
       <c r="G51"/>
       <c r="H51"/>
       <c r="I51"/>
       <c r="J51"/>
     </row>
-    <row r="52" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D52" s="1"/>
       <c r="G52"/>
       <c r="H52"/>
       <c r="I52"/>
       <c r="J52"/>
     </row>
-    <row r="53" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D53" s="1"/>
       <c r="G53"/>
       <c r="H53"/>
       <c r="I53"/>
       <c r="J53"/>
     </row>
-    <row r="54" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D54" s="1"/>
       <c r="G54"/>
       <c r="H54"/>
       <c r="I54"/>
       <c r="J54"/>
     </row>
-    <row r="55" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D55" s="1"/>
       <c r="G55"/>
       <c r="H55"/>
       <c r="I55"/>
       <c r="J55"/>
     </row>
-    <row r="56" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D56" s="1"/>
       <c r="G56"/>
       <c r="H56"/>
       <c r="I56"/>
       <c r="J56"/>
     </row>
-    <row r="57" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D57" s="1"/>
       <c r="G57"/>
       <c r="H57"/>
       <c r="I57"/>
       <c r="J57"/>
     </row>
-    <row r="58" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D58" s="1"/>
       <c r="G58"/>
       <c r="H58"/>
       <c r="I58"/>
       <c r="J58"/>
     </row>
-    <row r="59" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D59" s="1"/>
       <c r="G59"/>
       <c r="H59"/>
       <c r="I59"/>
       <c r="J59"/>
     </row>
-    <row r="60" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D60" s="1"/>
       <c r="G60"/>
       <c r="H60"/>
       <c r="I60"/>
       <c r="J60"/>
     </row>
-    <row r="61" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D61" s="1"/>
       <c r="G61"/>
       <c r="H61"/>
       <c r="I61"/>
       <c r="J61"/>
     </row>
-    <row r="62" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D62" s="1"/>
       <c r="G62"/>
       <c r="H62"/>
       <c r="I62"/>
       <c r="J62"/>
     </row>
-    <row r="63" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D63" s="1"/>
       <c r="G63"/>
       <c r="H63"/>
       <c r="I63"/>
       <c r="J63"/>
     </row>
-    <row r="64" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D64" s="1"/>
       <c r="G64"/>
       <c r="H64"/>
       <c r="I64"/>
       <c r="J64"/>
     </row>
-    <row r="65" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D65" s="1"/>
       <c r="G65"/>
       <c r="H65"/>
       <c r="I65"/>
       <c r="J65"/>
     </row>
-    <row r="66" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D66" s="1"/>
       <c r="G66"/>
       <c r="H66"/>
       <c r="I66"/>
       <c r="J66"/>
     </row>
-    <row r="67" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D67" s="1"/>
       <c r="G67"/>
       <c r="H67"/>
@@ -4417,16 +4438,16 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" style="3" customWidth="1"/>
-    <col min="3" max="3" width="86.7109375" style="3" customWidth="1"/>
-    <col min="4" max="5" width="10.85546875" style="3"/>
-    <col min="6" max="6" width="45.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="7.140625" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="86.6640625" style="3" customWidth="1"/>
+    <col min="4" max="5" width="10.88671875" style="3"/>
+    <col min="6" max="6" width="45.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="7.109375" customWidth="1"/>
+    <col min="8" max="8" width="15.109375" customWidth="1"/>
+    <col min="9" max="9" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4456,7 +4477,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D2" s="1"/>
       <c r="H2" s="69" t="s">
         <v>47</v>
@@ -4467,7 +4488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D3" s="1"/>
       <c r="H3" s="67" t="s">
         <v>48</v>
@@ -4478,7 +4499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D4" s="1"/>
       <c r="H4" s="67" t="s">
         <v>49</v>
@@ -4489,7 +4510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D5" s="1"/>
       <c r="H5" s="67" t="s">
         <v>50</v>
@@ -4500,7 +4521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D6" s="1"/>
       <c r="H6" s="71" t="s">
         <v>51</v>
@@ -4511,7 +4532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D7" s="1"/>
       <c r="H7" s="73" t="s">
         <v>52</v>
@@ -4533,10 +4554,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4550,7 +4571,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="H13" s="34" t="s">
         <v>28</v>
       </c>
@@ -4559,7 +4580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="H14" s="34" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Added Dictionary in main-class
</commit_message>
<xml_diff>
--- a/Dokumentation/Aquila_Zeitaufzeichnung.xlsx
+++ b/Dokumentation/Aquila_Zeitaufzeichnung.xlsx
@@ -1087,12 +1087,12 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:shape val="box"/>
-        <c:axId val="84070784"/>
-        <c:axId val="84072320"/>
+        <c:axId val="176767744"/>
+        <c:axId val="176769280"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="84070784"/>
+        <c:axId val="176767744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1101,7 +1101,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84072320"/>
+        <c:crossAx val="176769280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1109,7 +1109,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84072320"/>
+        <c:axId val="176769280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1125,7 +1125,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="84070784"/>
+        <c:crossAx val="176767744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1258,12 +1258,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="92170112"/>
-        <c:axId val="92171648"/>
+        <c:axId val="176781568"/>
+        <c:axId val="176783360"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="92170112"/>
+        <c:axId val="176781568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1272,7 +1272,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92171648"/>
+        <c:crossAx val="176783360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1280,7 +1280,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="92171648"/>
+        <c:axId val="176783360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1291,7 +1291,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92170112"/>
+        <c:crossAx val="176781568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1662,8 +1662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1699,7 +1699,7 @@
       </c>
       <c r="B3" s="10">
         <f>SUM(B6,B12,B17)</f>
-        <v>48.5</v>
+        <v>38.5</v>
       </c>
       <c r="C3" s="27">
         <v>1</v>
@@ -1798,7 +1798,7 @@
       </c>
       <c r="B12" s="19">
         <f>Software!J6</f>
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C12" s="29">
         <v>1</v>
@@ -1813,7 +1813,7 @@
       </c>
       <c r="B13" s="24">
         <f>Software!J2</f>
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C13" s="31"/>
       <c r="D13" s="32"/>
@@ -2459,7 +2459,7 @@
   <dimension ref="A1:J68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2525,7 +2525,7 @@
       <c r="I2" s="70"/>
       <c r="J2" s="4">
         <f>SUMIF(B:B,H2,E:E)</f>
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -2637,7 +2637,7 @@
       <c r="I6" s="68"/>
       <c r="J6" s="10">
         <f>SUM(J2:J5)</f>
-        <v>41</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -2701,44 +2701,10 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="D10" s="1">
-        <v>41316</v>
-      </c>
-      <c r="E10" s="3">
-        <v>5</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>162</v>
-      </c>
+      <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="D11" s="1">
-        <v>41316</v>
-      </c>
-      <c r="E11" s="3">
-        <v>5</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>162</v>
-      </c>
+      <c r="D11" s="1"/>
       <c r="H11" s="6" t="s">
         <v>5</v>
       </c>
@@ -2763,7 +2729,7 @@
       </c>
       <c r="I13" s="4">
         <f>SUMIF(A:A,H13,E:E)</f>
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2773,7 +2739,7 @@
       </c>
       <c r="I14" s="33">
         <f>SUMIF(A:A,H14,E:E)</f>
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -3758,7 +3724,7 @@
   <dimension ref="A1:J67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="A17" sqref="A17:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4069,7 +4035,7 @@
       </c>
       <c r="I12" s="41">
         <f>SUMIF(A:A,H12,E:E)</f>
-        <v>19.5</v>
+        <v>24.5</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4096,7 +4062,7 @@
       </c>
       <c r="I13" s="39">
         <f>SUMIF(A:A,H13,E:E)</f>
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -4163,112 +4129,146 @@
       <c r="I16"/>
       <c r="J16"/>
     </row>
-    <row r="17" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D17" s="1"/>
+    <row r="17" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D17" s="1">
+        <v>41316</v>
+      </c>
+      <c r="E17" s="3">
+        <v>5</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>162</v>
+      </c>
       <c r="G17"/>
       <c r="H17"/>
       <c r="I17"/>
       <c r="J17"/>
     </row>
-    <row r="18" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D18" s="1"/>
+    <row r="18" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D18" s="1">
+        <v>41316</v>
+      </c>
+      <c r="E18" s="3">
+        <v>5</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>162</v>
+      </c>
       <c r="G18"/>
       <c r="H18"/>
       <c r="I18"/>
       <c r="J18"/>
     </row>
-    <row r="19" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D19" s="1"/>
       <c r="G19"/>
       <c r="H19"/>
       <c r="I19"/>
       <c r="J19"/>
     </row>
-    <row r="20" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D20" s="1"/>
       <c r="G20"/>
       <c r="H20"/>
       <c r="I20"/>
       <c r="J20"/>
     </row>
-    <row r="21" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D21" s="1"/>
       <c r="G21"/>
       <c r="H21"/>
       <c r="I21"/>
       <c r="J21"/>
     </row>
-    <row r="22" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D22" s="1"/>
       <c r="G22"/>
       <c r="H22"/>
       <c r="I22"/>
       <c r="J22"/>
     </row>
-    <row r="23" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D23" s="1"/>
       <c r="G23"/>
       <c r="H23"/>
       <c r="I23"/>
       <c r="J23"/>
     </row>
-    <row r="24" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D24" s="1"/>
       <c r="G24"/>
       <c r="H24"/>
       <c r="I24"/>
       <c r="J24"/>
     </row>
-    <row r="25" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D25" s="1"/>
       <c r="G25"/>
       <c r="H25"/>
       <c r="I25"/>
       <c r="J25"/>
     </row>
-    <row r="26" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D26" s="1"/>
       <c r="G26"/>
       <c r="H26"/>
       <c r="I26"/>
       <c r="J26"/>
     </row>
-    <row r="27" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D27" s="1"/>
       <c r="G27"/>
       <c r="H27"/>
       <c r="I27"/>
       <c r="J27"/>
     </row>
-    <row r="28" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D28" s="1"/>
       <c r="G28"/>
       <c r="H28"/>
       <c r="I28"/>
       <c r="J28"/>
     </row>
-    <row r="29" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D29" s="1"/>
       <c r="G29"/>
       <c r="H29"/>
       <c r="I29"/>
       <c r="J29"/>
     </row>
-    <row r="30" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D30" s="1"/>
       <c r="G30"/>
       <c r="H30"/>
       <c r="I30"/>
       <c r="J30"/>
     </row>
-    <row r="31" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D31" s="1"/>
       <c r="G31"/>
       <c r="H31"/>
       <c r="I31"/>
       <c r="J31"/>
     </row>
-    <row r="32" spans="4:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D32" s="1"/>
       <c r="G32"/>
       <c r="H32"/>
@@ -4528,12 +4528,18 @@
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="H5:I5"/>
   </mergeCells>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A17:A22 A49:A1048576 A41:A46 A29:A39 A24:A26 A2:A15">
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A15 A49:A1048576 A41:A46 A29:A39 A24:A26 A19:A22">
       <formula1>$H$11:$H$13</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B48:B1048576 B24:B26 B28:B38 B40:B45 B1:B22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B48:B1048576 B24:B26 B28:B38 B40:B45 B1:B16 B19:B22">
       <formula1>$H$2:$H$4</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17:B18">
+      <formula1>$H$2:$H$5</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A17:A18">
+      <formula1>$H$12:$H$14</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>